<commit_message>
defined entity and training data for transfer admission, added sparse matrix for rest of freshman profile. Rewrote backend algorithm to return a list of answers
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9B96AE-4CB8-4219-B723-63BA94C23C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BC629A-82E1-4906-97E2-27F73F6301C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basis For Selection" sheetId="1" r:id="rId1"/>
     <sheet name="Freshman Profile_Percentile" sheetId="2" r:id="rId2"/>
+    <sheet name="Freshman Profile_SAT ACT Score " sheetId="3" r:id="rId3"/>
+    <sheet name="Freshman Profile_Class Rank GPA" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="146">
   <si>
     <t>Answer</t>
   </si>
@@ -227,6 +229,243 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 200-299 range for sat evidence-based reading and writing</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 200-299 range for sat math</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 300-399 range for sat evidence-based reading and writing</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 300-399 range for sat math</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 700-800 range for sat evidence-based reading and writing</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 700-800 range for sat math</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 600-699 range for sat evidence-based reading and writing</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 600-699 range for sat math</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 500-599 range for sat evidence-based reading and writing</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 500-599 range for sat math</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 400-499 range for sat evidence-based reading and writing</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 400-499 range for sat math</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 1400-1600 range for sat composite</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 1200-1399 range for sat composite</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 1000-1199 range for sat composite    </t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 800-999 range for sat composite</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 600-799 range for sat composite</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with sat score in the 400-599 range for sat composite</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range 30-36 for act composite</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range 30-36 for act english</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range 30-36 for act math</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range 24-29 for act composite</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range 24-29 for act english</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range 24-29 for act math</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range 18-23 for act composite</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range 18-23 for act english</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range 18-23 for act math</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range 12-17 for act composite</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range 12-17 for act english</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range 12-17 for act math </t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range 6-11 for act composite</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range 6-11 for act english</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range 6-11 for act math</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range below 6 for act composite</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range below 6 for act english</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range below 6 for act math</t>
+  </si>
+  <si>
+    <t>What is the percentage of students in the bottom half of their high school graduating class?</t>
+  </si>
+  <si>
+    <t>What is the percentage of students in the bottom quarter of their high school graduating class?</t>
+  </si>
+  <si>
+    <t>What is the percentage of students in the top half of their high school graduating class?</t>
+  </si>
+  <si>
+    <t>What is the percentage of students in the top quarter of their high school graduating class?</t>
+  </si>
+  <si>
+    <t>What is the percentage of students in the top tenth of their high school graduating class?</t>
+  </si>
+  <si>
+    <t>What is the percentage of students who submitted high school class rank?</t>
+  </si>
+  <si>
+    <t>What is the percentage of students with gpa between 4.00?</t>
+  </si>
+  <si>
+    <t>What is the percentage of students with gpa between 3.75 and 3.99?</t>
+  </si>
+  <si>
+    <t>What is the percentage of students with gpa between 3.50 and 3.74?</t>
+  </si>
+  <si>
+    <t>What is the percentage of students with gpa between 3.25 and 3.49?</t>
+  </si>
+  <si>
+    <t>What is the percentage of students with gpa between 3.00 and 3.24?</t>
+  </si>
+  <si>
+    <t>What is the percentage of students with gpa between 2.50 and 2.99?</t>
+  </si>
+  <si>
+    <t>What is the percentage of students with gpa between 2.00 and 2.49?</t>
+  </si>
+  <si>
+    <t>What is the percentage of students with gpa between 1.00 and 1.99?</t>
+  </si>
+  <si>
+    <t>What is the percentage of students with gpa between below 1.00?</t>
+  </si>
+  <si>
+    <t>What is the average high school gpa for students who submitted gpa?</t>
+  </si>
+  <si>
+    <t>60.1% (303/504)</t>
+  </si>
+  <si>
+    <t>22.6% (114/504)</t>
+  </si>
+  <si>
+    <t>11.5% (58/504)</t>
+  </si>
+  <si>
+    <t>4.4% (22/504)</t>
+  </si>
+  <si>
+    <t>1.2% (6/504)</t>
+  </si>
+  <si>
+    <t>0.2% (1/504)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  What is the percentage of students who submitted gpa?</t>
+  </si>
+  <si>
+    <t>94.9 % (504/531)</t>
+  </si>
+  <si>
+    <t>27.1%</t>
+  </si>
+  <si>
+    <t>54%</t>
+  </si>
+  <si>
+    <t>38.3%</t>
+  </si>
+  <si>
+    <t>18.9%</t>
+  </si>
+  <si>
+    <t>7.7%</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>39.7%</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>10.3%</t>
+  </si>
+  <si>
+    <t>63.2%</t>
+  </si>
+  <si>
+    <t>60.1%</t>
+  </si>
+  <si>
+    <t>61.5%</t>
+  </si>
+  <si>
+    <t>30.7%</t>
+  </si>
+  <si>
+    <t>29.1%</t>
+  </si>
+  <si>
+    <t>37.5%</t>
+  </si>
+  <si>
+    <t>6.1%</t>
+  </si>
+  <si>
+    <t>10.1%</t>
+  </si>
+  <si>
+    <t>10%</t>
+  </si>
+  <si>
+    <t>0.7%</t>
   </si>
 </sst>
 </file>
@@ -274,12 +513,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,21 +984,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3892E9F-E7EA-42B9-AE4C-1275BBD6A387}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="81.21875" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
@@ -764,7 +1006,7 @@
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>350</v>
       </c>
     </row>
@@ -772,7 +1014,7 @@
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>296</v>
       </c>
     </row>
@@ -780,7 +1022,7 @@
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>64</v>
       </c>
     </row>
@@ -788,7 +1030,7 @@
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>65</v>
       </c>
     </row>
@@ -796,7 +1038,7 @@
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>1270</v>
       </c>
     </row>
@@ -804,7 +1046,7 @@
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="5">
         <v>610</v>
       </c>
     </row>
@@ -812,7 +1054,7 @@
       <c r="A8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>650</v>
       </c>
     </row>
@@ -820,7 +1062,7 @@
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>66</v>
       </c>
     </row>
@@ -828,7 +1070,7 @@
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>1355</v>
       </c>
     </row>
@@ -836,7 +1078,7 @@
       <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="5">
         <v>650</v>
       </c>
     </row>
@@ -844,7 +1086,7 @@
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <v>700</v>
       </c>
     </row>
@@ -852,7 +1094,7 @@
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>66</v>
       </c>
     </row>
@@ -860,7 +1102,7 @@
       <c r="A14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="5">
         <v>1440</v>
       </c>
     </row>
@@ -868,7 +1110,7 @@
       <c r="A15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="5">
         <v>700</v>
       </c>
     </row>
@@ -876,7 +1118,7 @@
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="5">
         <v>760</v>
       </c>
     </row>
@@ -884,7 +1126,7 @@
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="5">
         <v>1352</v>
       </c>
     </row>
@@ -892,7 +1134,7 @@
       <c r="A18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="5">
         <v>1352</v>
       </c>
     </row>
@@ -900,7 +1142,7 @@
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="5">
         <v>652</v>
       </c>
     </row>
@@ -908,7 +1150,7 @@
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="5">
         <v>700</v>
       </c>
     </row>
@@ -916,7 +1158,7 @@
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>66</v>
       </c>
     </row>
@@ -924,7 +1166,7 @@
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="5">
         <v>27</v>
       </c>
     </row>
@@ -932,7 +1174,7 @@
       <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="5">
         <v>28</v>
       </c>
     </row>
@@ -940,7 +1182,7 @@
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="5">
         <v>26</v>
       </c>
     </row>
@@ -948,7 +1190,7 @@
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="5" t="s">
         <v>66</v>
       </c>
     </row>
@@ -956,7 +1198,7 @@
       <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="5">
         <v>31</v>
       </c>
     </row>
@@ -964,7 +1206,7 @@
       <c r="A27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="5">
         <v>31</v>
       </c>
     </row>
@@ -972,7 +1214,7 @@
       <c r="A28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="5">
         <v>31.5</v>
       </c>
     </row>
@@ -980,7 +1222,7 @@
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="5" t="s">
         <v>66</v>
       </c>
     </row>
@@ -988,7 +1230,7 @@
       <c r="A30" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="5">
         <v>33</v>
       </c>
     </row>
@@ -996,7 +1238,7 @@
       <c r="A31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="5">
         <v>34</v>
       </c>
     </row>
@@ -1004,7 +1246,7 @@
       <c r="A32" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="5">
         <v>35</v>
       </c>
     </row>
@@ -1012,7 +1254,7 @@
       <c r="A33" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="5" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1020,7 +1262,7 @@
       <c r="A34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="5">
         <v>30</v>
       </c>
     </row>
@@ -1028,7 +1270,7 @@
       <c r="A35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="5">
         <v>30</v>
       </c>
     </row>
@@ -1036,7 +1278,7 @@
       <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="5">
         <v>30</v>
       </c>
     </row>
@@ -1044,7 +1286,7 @@
       <c r="A37" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="5" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1055,4 +1297,487 @@
     <ignoredError sqref="B4:B5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C307D05E-B833-4D75-9855-8E27A1B5E2C9}">
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="114.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="B8" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB852AE-A4C7-4284-9FBD-1CEEB9311916}">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="87.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="5">
+        <v>4.0199999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added sparse matrix and training data for transfer admission
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BC629A-82E1-4906-97E2-27F73F6301C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DC7DD3-A13A-44FF-BD7A-C1068B52432F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basis For Selection" sheetId="1" r:id="rId1"/>
     <sheet name="Freshman Profile_Percentile" sheetId="2" r:id="rId2"/>
     <sheet name="Freshman Profile_SAT ACT Score " sheetId="3" r:id="rId3"/>
     <sheet name="Freshman Profile_Class Rank GPA" sheetId="4" r:id="rId4"/>
+    <sheet name="Transfer Admission_General" sheetId="5" r:id="rId5"/>
+    <sheet name="Transfer Admission_Policies" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="196">
   <si>
     <t>Answer</t>
   </si>
@@ -466,6 +468,156 @@
   </si>
   <si>
     <t>0.7%</t>
+  </si>
+  <si>
+    <t>66%</t>
+  </si>
+  <si>
+    <t>91%</t>
+  </si>
+  <si>
+    <t>99%</t>
+  </si>
+  <si>
+    <t>1%</t>
+  </si>
+  <si>
+    <t>46%</t>
+  </si>
+  <si>
+    <t>May transfer students earn advanced standing credit by transferring credits earned from course work completed at other colleges/universities?</t>
+  </si>
+  <si>
+    <t>Does Rose-Hulman enroll transfer students</t>
+  </si>
+  <si>
+    <t>How many male transfer applicants applied?</t>
+  </si>
+  <si>
+    <t>How many male transfer applicants are admitted</t>
+  </si>
+  <si>
+    <t>How many male transfer applicants are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female transfer applicants applied?</t>
+  </si>
+  <si>
+    <t>How many female transfer applicants are admitted</t>
+  </si>
+  <si>
+    <t>How many female transfer applicants are enrolled?</t>
+  </si>
+  <si>
+    <t>At which term may transfer students enroll</t>
+  </si>
+  <si>
+    <t>Does Rose-Hulman require high school transcript to apply for transfer admission?</t>
+  </si>
+  <si>
+    <t>Does Rose-Hulman require college transcript to apply for transfer admission?</t>
+  </si>
+  <si>
+    <t>Does Rose-Hulman require essay to apply for transfer admission?</t>
+  </si>
+  <si>
+    <t>Does Rose-Hulman require interview to apply for transfer admission?</t>
+  </si>
+  <si>
+    <t>Does Rose-Hulman require standardized test score to apply for transfer admission?</t>
+  </si>
+  <si>
+    <t>Does Rose-Hulman require statement of good standing to apply for transfer admission?</t>
+  </si>
+  <si>
+    <t>What is the minimum high school grade point average required  of transfer applicants?</t>
+  </si>
+  <si>
+    <t>What is the minimum college grade point average required of transfer applicants?</t>
+  </si>
+  <si>
+    <t>When does Rose-Hulman review transfer student applications?</t>
+  </si>
+  <si>
+    <t>Does an open admission policy apply to transfer students?</t>
+  </si>
+  <si>
+    <t>Are there any additional requirements for transfer admission?</t>
+  </si>
+  <si>
+    <t>What is the lowest grade earn for any course that maybe transferred for credit</t>
+  </si>
+  <si>
+    <t>What is the minimum number of credits that transfer students must complete to earn a associates degree</t>
+  </si>
+  <si>
+    <t>What is the minimum number of credits that transfer students must complete to earn a bachelor degree</t>
+  </si>
+  <si>
+    <t>Are there any additional transfer credit policies?</t>
+  </si>
+  <si>
+    <t>Rose-Hulman does enroll transfer students</t>
+  </si>
+  <si>
+    <t>Students may earn advanced standing credit by transferring credit earned from course work completed at other college/university</t>
+  </si>
+  <si>
+    <t>Transfer students may enroll during the fall term.</t>
+  </si>
+  <si>
+    <t>No, transfer students do not need to have minimum number of credit completed</t>
+  </si>
+  <si>
+    <t>Does a transfer applicant need to have minimum number of credits completed or else they must apply as an entering freshman? If so what is the minimum credit and the unit of measure?</t>
+  </si>
+  <si>
+    <t>Essays or personal statement is required for transfer admission.</t>
+  </si>
+  <si>
+    <t>College transcript is required  for transfer admission.</t>
+  </si>
+  <si>
+    <t>High school transcript is recommended of some for transfer admission.</t>
+  </si>
+  <si>
+    <t>Interview is recommended of some to apply for transfer admission</t>
+  </si>
+  <si>
+    <t>Standarized test score is not required</t>
+  </si>
+  <si>
+    <t>Statement of good standing from prior institutions is recommended of all transfer applicants.</t>
+  </si>
+  <si>
+    <t>There is no minimum high school gpa requirement for transfer admission</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>Rose-Hulman review transfer applications on a rolling basis (year round).</t>
+  </si>
+  <si>
+    <t>No, open admission policy does not apply to students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students must have a semester of calculus, as well as calculus-based physics and chemistry. </t>
+  </si>
+  <si>
+    <t>The lowest grade earned from any course that may be transferred for credit is C or 2.0</t>
+  </si>
+  <si>
+    <t>What is the maximum number of credit that maybe transferred from a 2-year institution</t>
+  </si>
+  <si>
+    <t>What is the maximum number of credit that maybe transferred from a 4-year institution</t>
+  </si>
+  <si>
+    <t>Rose-Hulman does not offer associate degree</t>
+  </si>
+  <si>
+    <t>Credits to be transferred are reviewed by each department and the final decision to award credit is up to the appropriate department chairs.</t>
   </si>
 </sst>
 </file>
@@ -513,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -522,6 +674,15 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,7 +966,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -985,7 +1146,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1304,7 +1465,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1622,8 +1783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB852AE-A4C7-4284-9FBD-1CEEB9311916}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1644,48 +1805,48 @@
       <c r="A2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="5">
-        <v>0.66</v>
+      <c r="B2" s="5" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="5">
-        <v>0.91</v>
+      <c r="B3" s="5" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="5">
-        <v>0.99</v>
+      <c r="B4" s="5" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="5">
-        <v>0.01</v>
+      <c r="B5" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="5">
-        <v>0</v>
+      <c r="B6" s="5" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="5">
-        <v>0.46</v>
+      <c r="B7" s="5" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1740,24 +1901,24 @@
       <c r="A14" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B14" s="5">
-        <v>0</v>
+      <c r="B14" s="5" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B15" s="5">
-        <v>0</v>
+      <c r="B15" s="5" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B16" s="5">
-        <v>0</v>
+      <c r="B16" s="5" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -1774,6 +1935,280 @@
       </c>
       <c r="B18" s="5" t="s">
         <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CD6236-1D5E-43C4-8447-268AAEF1A0C5}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="131" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="7">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF4F714-5A64-4B0A-90E7-28D299FDF6BE}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="96.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.88671875" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B4" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
defined entities and added training data for student life section
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DC7DD3-A13A-44FF-BD7A-C1068B52432F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C6AD3E-4739-4C29-8AD7-8D49CE4C6FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,9 +566,6 @@
     <t>Transfer students may enroll during the fall term.</t>
   </si>
   <si>
-    <t>No, transfer students do not need to have minimum number of credit completed</t>
-  </si>
-  <si>
     <t>Does a transfer applicant need to have minimum number of credits completed or else they must apply as an entering freshman? If so what is the minimum credit and the unit of measure?</t>
   </si>
   <si>
@@ -618,6 +615,9 @@
   </si>
   <si>
     <t>Credits to be transferred are reviewed by each department and the final decision to award credit is up to the appropriate department chairs.</t>
+  </si>
+  <si>
+    <t>Transfer students do not need to have minimum number of credit completed</t>
   </si>
 </sst>
 </file>
@@ -1948,7 +1948,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2039,10 +2039,10 @@
     </row>
     <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -2050,7 +2050,7 @@
         <v>160</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2058,7 +2058,7 @@
         <v>161</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -2066,7 +2066,7 @@
         <v>162</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -2074,7 +2074,7 @@
         <v>163</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -2082,7 +2082,7 @@
         <v>164</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -2090,7 +2090,7 @@
         <v>165</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -2098,7 +2098,7 @@
         <v>166</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -2106,7 +2106,7 @@
         <v>167</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -2114,7 +2114,7 @@
         <v>168</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -2122,7 +2122,7 @@
         <v>169</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -2130,7 +2130,7 @@
         <v>170</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -2168,12 +2168,12 @@
         <v>171</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B3" s="6">
         <v>90</v>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B4" s="6">
         <v>90</v>
@@ -2192,7 +2192,7 @@
         <v>172</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2208,7 +2208,7 @@
         <v>174</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated domain to contain newest entity and updated cds answer
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C6AD3E-4739-4C29-8AD7-8D49CE4C6FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA6442E-2FE4-418A-B755-43B1CF418B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basis For Selection" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Freshman Profile_Class Rank GPA" sheetId="4" r:id="rId4"/>
     <sheet name="Transfer Admission_General" sheetId="5" r:id="rId5"/>
     <sheet name="Transfer Admission_Policies" sheetId="6" r:id="rId6"/>
+    <sheet name="Student Life_Categories" sheetId="7" r:id="rId7"/>
+    <sheet name="Student Life_Offered" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="237">
   <si>
     <t>Answer</t>
   </si>
@@ -618,6 +620,129 @@
   </si>
   <si>
     <t>Transfer students do not need to have minimum number of credit completed</t>
+  </si>
+  <si>
+    <t>What is the percentage of full-time and part-time first year first time freshman students who are out of state?</t>
+  </si>
+  <si>
+    <t>What is the percentage of full-time and part-time undergraduate students who are out of state?</t>
+  </si>
+  <si>
+    <t>What is the percentage of full-time and part-time undergraduate students who joined fraternities?</t>
+  </si>
+  <si>
+    <t>What is the percentage of full-time and part-time first year first time students who joined fraternities?</t>
+  </si>
+  <si>
+    <t>What is the percentage of full-time and part-time first year first time freshman students who joined sororities?</t>
+  </si>
+  <si>
+    <t>What is the percentage of full-time and part-time undergraduate students who joined sororities</t>
+  </si>
+  <si>
+    <t>What is the percentage of full-time and part-time first year first time freshman students who live in college owned, operated, or affiliated housing?</t>
+  </si>
+  <si>
+    <t>What is the percentage of full-time and part-time undergraduate students who live in college owned, operated, or affiliated housing?</t>
+  </si>
+  <si>
+    <t>70.7%</t>
+  </si>
+  <si>
+    <t>66.1%</t>
+  </si>
+  <si>
+    <t>22.9%</t>
+  </si>
+  <si>
+    <t>32.5%</t>
+  </si>
+  <si>
+    <t>93.0%</t>
+  </si>
+  <si>
+    <t>57.8%</t>
+  </si>
+  <si>
+    <t>7.0%</t>
+  </si>
+  <si>
+    <t>42.2%</t>
+  </si>
+  <si>
+    <t>35.5%</t>
+  </si>
+  <si>
+    <t>0.2%</t>
+  </si>
+  <si>
+    <t>What is the percentage of full-time and part-time first year first time freshman students who live off campus or commute?</t>
+  </si>
+  <si>
+    <t>What is the percentage of full-time and part-time undergraduate students who live off campus or commute?</t>
+  </si>
+  <si>
+    <t>What is the percentage of full-time and part-time first year first time freshman students who are age 25 and older?</t>
+  </si>
+  <si>
+    <t>0.4%</t>
+  </si>
+  <si>
+    <t>What is the average age of both full-time and part-time first year first time freshman students</t>
+  </si>
+  <si>
+    <t>What is percentage of full-time and part-time undergraduate students who are age 25 and older</t>
+  </si>
+  <si>
+    <t>What is the average age of only full-time first year first time freshman students?</t>
+  </si>
+  <si>
+    <t>What is the average age of only full-time undergraduate students?</t>
+  </si>
+  <si>
+    <t>What is the average age of both full-time and part-time undergraduate students</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>String Answer?</t>
+  </si>
+  <si>
+    <t>The average age of full-time undergraduate student is 19.7</t>
+  </si>
+  <si>
+    <t>The average age of full-time freshman students is 18.1</t>
+  </si>
+  <si>
+    <t>The average age of all (full-time and part-time) freshman students is 18.1</t>
+  </si>
+  <si>
+    <t>The average age of all (full-time and part-time) undergraduate students is 18.1</t>
+  </si>
+  <si>
+    <t>What extracurricular activities does Rose-Hulman offer?</t>
+  </si>
+  <si>
+    <t>Does Rose-Hulman offer army rotc ?</t>
+  </si>
+  <si>
+    <t>Does Rose-Hulman offer naval rotc ?</t>
+  </si>
+  <si>
+    <t>What type of college-owned, -operated, or -affiliated housing is available at Rose-Hulman?</t>
+  </si>
+  <si>
+    <t>The activities that Rose-Hulman offers include the following: campus ministries, choral groups, concert bands, dance, drama/theater, international student organizations, jazz band, music ensembles, musical theater, pep band, radio station, student governement, student newspaper, and symphony orchestra</t>
+  </si>
+  <si>
+    <t>Army ROTC is offerd on campus</t>
+  </si>
+  <si>
+    <t>Naval ROTC is not offered at Rose-Hulman</t>
+  </si>
+  <si>
+    <t>Does Rose-Hulman offer air force rotc ?</t>
   </si>
 </sst>
 </file>
@@ -1947,7 +2072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CD6236-1D5E-43C4-8447-268AAEF1A0C5}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2146,20 +2271,20 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="96.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.88671875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="35.88671875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2167,7 +2292,7 @@
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>190</v>
       </c>
     </row>
@@ -2175,7 +2300,7 @@
       <c r="A3" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="7">
         <v>90</v>
       </c>
     </row>
@@ -2183,7 +2308,7 @@
       <c r="A4" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="7">
         <v>90</v>
       </c>
     </row>
@@ -2191,7 +2316,7 @@
       <c r="A5" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2199,7 +2324,7 @@
       <c r="A6" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="7">
         <v>45</v>
       </c>
     </row>
@@ -2207,7 +2332,7 @@
       <c r="A7" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2215,4 +2340,236 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AECD6F-4371-4391-B58E-E510CF964736}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="131.44140625" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C15" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C16" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C17" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD4CE82-100F-475B-B66F-A9CBAA32385B}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="83.21875" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added test for student life and freshman profile
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA6442E-2FE4-418A-B755-43B1CF418B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B8B1B5-AA84-4D91-8410-9773B102D475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basis For Selection" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="239">
   <si>
     <t>Answer</t>
   </si>
@@ -322,9 +322,6 @@
     <t>What is the percentage of freshman students with act score in the range 12-17 for act english</t>
   </si>
   <si>
-    <t>What is the percentage of freshman students with act score in the range 12-17 for act math </t>
-  </si>
-  <si>
     <t>What is the percentage of freshman students with act score in the range 6-11 for act composite</t>
   </si>
   <si>
@@ -730,9 +727,6 @@
     <t>Does Rose-Hulman offer naval rotc ?</t>
   </si>
   <si>
-    <t>What type of college-owned, -operated, or -affiliated housing is available at Rose-Hulman?</t>
-  </si>
-  <si>
     <t>The activities that Rose-Hulman offers include the following: campus ministries, choral groups, concert bands, dance, drama/theater, international student organizations, jazz band, music ensembles, musical theater, pep band, radio station, student governement, student newspaper, and symphony orchestra</t>
   </si>
   <si>
@@ -743,6 +737,18 @@
   </si>
   <si>
     <t>Does Rose-Hulman offer air force rotc ?</t>
+  </si>
+  <si>
+    <t>Air Force ROTC is offered on campus</t>
+  </si>
+  <si>
+    <t>The type of college-owned, -operated, or -affiliated housing available include the following: coed dorms, men's dorms, apartment for single students, fraternity/sorority housing, and theme housing</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with act score in the range 12-17 for act math</t>
+  </si>
+  <si>
+    <t>What type of college owned, operated, or affiliated housing is available at Rose-Hulman?</t>
   </si>
 </sst>
 </file>
@@ -1268,27 +1274,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3892E9F-E7EA-42B9-AE4C-1275BBD6A387}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="81.21875" customWidth="1"/>
     <col min="2" max="2" width="31.44140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -1296,7 +1306,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -1304,23 +1314,23 @@
         <v>296</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
@@ -1328,7 +1338,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
@@ -1336,7 +1346,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>39</v>
       </c>
@@ -1344,7 +1354,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -1352,7 +1362,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -1360,7 +1370,7 @@
         <v>1355</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
@@ -1368,7 +1378,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
@@ -1376,7 +1386,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
@@ -1384,7 +1394,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>51</v>
       </c>
@@ -1392,7 +1402,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>53</v>
       </c>
@@ -1400,7 +1410,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
@@ -1579,9 +1589,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="B4:B5" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1589,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C307D05E-B833-4D75-9855-8E27A1B5E2C9}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1612,7 +1619,7 @@
         <v>71</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1620,7 +1627,7 @@
         <v>72</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1628,7 +1635,7 @@
         <v>73</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1636,7 +1643,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1644,7 +1651,7 @@
         <v>75</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1652,7 +1659,7 @@
         <v>76</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1660,7 +1667,7 @@
         <v>77</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1668,7 +1675,7 @@
         <v>78</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1676,7 +1683,7 @@
         <v>69</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1684,7 +1691,7 @@
         <v>70</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -1692,7 +1699,7 @@
         <v>67</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -1700,7 +1707,7 @@
         <v>68</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -1708,7 +1715,7 @@
         <v>79</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -1716,7 +1723,7 @@
         <v>80</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -1724,7 +1731,7 @@
         <v>81</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -1732,7 +1739,7 @@
         <v>82</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1740,7 +1747,7 @@
         <v>83</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -1748,7 +1755,7 @@
         <v>84</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1756,7 +1763,7 @@
         <v>85</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -1764,7 +1771,7 @@
         <v>86</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -1772,7 +1779,7 @@
         <v>87</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -1780,7 +1787,7 @@
         <v>88</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -1788,7 +1795,7 @@
         <v>89</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -1796,7 +1803,7 @@
         <v>90</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -1804,7 +1811,7 @@
         <v>91</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1812,7 +1819,7 @@
         <v>92</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -1820,7 +1827,7 @@
         <v>93</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -1828,7 +1835,7 @@
         <v>94</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -1836,63 +1843,63 @@
         <v>95</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>96</v>
+        <v>237</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1928,127 +1935,127 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B17" s="5">
         <v>4.0199999999999996</v>
@@ -2056,10 +2063,10 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2072,8 +2079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CD6236-1D5E-43C4-8447-268AAEF1A0C5}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2092,23 +2099,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4" s="7">
         <v>59</v>
@@ -2116,7 +2123,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B5" s="7">
         <v>30</v>
@@ -2124,7 +2131,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B6" s="7">
         <v>9</v>
@@ -2132,7 +2139,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B7" s="7">
         <v>23</v>
@@ -2140,7 +2147,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B8" s="7">
         <v>13</v>
@@ -2148,7 +2155,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B9" s="7">
         <v>2</v>
@@ -2156,106 +2163,106 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -2290,15 +2297,15 @@
     </row>
     <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B3" s="7">
         <v>90</v>
@@ -2306,7 +2313,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B4" s="7">
         <v>90</v>
@@ -2314,15 +2321,15 @@
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B6" s="7">
         <v>45</v>
@@ -2330,10 +2337,10 @@
     </row>
     <row r="7" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2347,7 +2354,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2365,147 +2372,147 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" t="s">
         <v>222</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="C17" t="s">
-        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2515,58 +2522,83 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD4CE82-100F-475B-B66F-A9CBAA32385B}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="83.21875" customWidth="1"/>
     <col min="2" max="2" width="47.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B3" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="C4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="B5" s="6" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="C5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>232</v>
+      <c r="C6" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added cohort questions to ExcelInput
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B0DF82-F195-4DAB-9634-0D4ED11E4D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D1B74D-BEBE-40B6-B916-27ACA34E8324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basis For Selection" sheetId="1" r:id="rId1"/>
-    <sheet name="Admission Policies" sheetId="9" r:id="rId2"/>
-    <sheet name="Freshman Profile_Percentile" sheetId="2" r:id="rId3"/>
-    <sheet name="Freshman Profile_SAT ACT Score " sheetId="3" r:id="rId4"/>
-    <sheet name="Freshman Profile_Class Rank GPA" sheetId="4" r:id="rId5"/>
-    <sheet name="Transfer Admission_General" sheetId="5" r:id="rId6"/>
-    <sheet name="Transfer Admission_Policies" sheetId="6" r:id="rId7"/>
-    <sheet name="Student Life_Categories" sheetId="7" r:id="rId8"/>
-    <sheet name="Student Life_Offered" sheetId="8" r:id="rId9"/>
+    <sheet name="Cohort" sheetId="10" r:id="rId2"/>
+    <sheet name="Admission Policies" sheetId="9" r:id="rId3"/>
+    <sheet name="Freshman Profile_Percentile" sheetId="2" r:id="rId4"/>
+    <sheet name="Freshman Profile_SAT ACT Score " sheetId="3" r:id="rId5"/>
+    <sheet name="Freshman Profile_Class Rank GPA" sheetId="4" r:id="rId6"/>
+    <sheet name="Transfer Admission_General" sheetId="5" r:id="rId7"/>
+    <sheet name="Transfer Admission_Policies" sheetId="6" r:id="rId8"/>
+    <sheet name="Student Life_Categories" sheetId="7" r:id="rId9"/>
+    <sheet name="Student Life_Offered" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="303">
   <si>
     <t>Answer</t>
   </si>
@@ -820,6 +821,129 @@
   </si>
   <si>
     <t>Rose-Hulman does have early action. The early action closing date is November 1st and early action notification date is December 15th. Students can still apply to other early action programs after applying for early action at Rose-Hulman.</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>How many students in the initial cohort were recipients of a Federal Pell Grant?</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>How many of those students in the initial cohort were recipients of a Subsidized Stafford Loan but not a Pell Grant?</t>
+  </si>
+  <si>
+    <t>199</t>
+  </si>
+  <si>
+    <t>How many of those students in the initial cohort did not receive either a Pell Grant or a subsidized Stafford Loan?</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>How many exempted student were recipients of a Federal Pell Grant?</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>How many of exempted students were recipients of a Subsidized Stafford Loan but not a Pell Grant?</t>
+  </si>
+  <si>
+    <t>How many of exempted students did not receive a Pell Grant or a subsidized Stafford Loan?</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>How many students in the final cohort were recipients of a Federal Pell Grant?</t>
+  </si>
+  <si>
+    <t>How many students in the final cohort were recipients of a Subsidized Stafford Loan but not a Pell Grant?</t>
+  </si>
+  <si>
+    <t>How many students in the final cohort did not receive a Pell Grant or a subsidized Stafford Loan?</t>
+  </si>
+  <si>
+    <t>299</t>
+  </si>
+  <si>
+    <t>How many students in the initial cohort completed the program within four years and were recipients of a Federal Pell Grant?</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>How many students in the initial cohort who completed the program within four years were recipients of a Subsidized Stafford Loan but not a Pell Grant?</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>How many students in the initial cohort who completed the program within four years but did not receive a Pell Grant or a subsidized Stafford Loan?</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>How many students  in the initial cohort who completed the program in between four and five years were recipients of a Federal Pell Grant?</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>How many students  in the initial cohort who completed the program in between four and five years were recipients of a Subsidized Stafford Loan but not a Pell Grant?</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>How many students in the initial cohort who completed the program in between four and five years did not receive a Pell Grant or a subsidized Stafford Loan?</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>How many students who completed the program between five and six years were recipients of a Federal Pell Grant?</t>
+  </si>
+  <si>
+    <t>How many students who completed the program between five and six years were recipients of a Subsidized Stafford Loan but not a Pell Grant?</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>How many students who completed the program between five and six years did not receive a Pell Grant or a subsidized Stafford Loan?</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>Operation Allowed?</t>
+  </si>
+  <si>
+    <t>Sum up?</t>
+  </si>
+  <si>
+    <t>Answer Range?</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The {aggregation} of students {range} in the {initial_final} {year} cohort {} is {value} </t>
+  </si>
+  <si>
+    <t>For student cohort data, you can ask about students exemptions from a cohort year, number of students who graduated within four, five, or six year and graduation rate for those years. You can also ask all of the things paired with financial aid in terms of student who received pell-grant, student who received stafford loan but not pell grant and student who received neither.</t>
   </si>
 </sst>
 </file>
@@ -867,7 +991,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -880,6 +1004,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1168,7 +1299,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1343,12 +1474,318 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD4CE82-100F-475B-B66F-A9CBAA32385B}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="83.21875" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7606B2B-8397-4A8E-AF38-C293D77D8867}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="78.33203125" customWidth="1"/>
+    <col min="2" max="2" width="72.33203125" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0908D19-61E8-460E-9695-3943D19E115C}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="58.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1494,12 +1931,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3892E9F-E7EA-42B9-AE4C-1275BBD6A387}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="AG26" zoomScale="105" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1814,7 +2251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C307D05E-B833-4D75-9855-8E27A1B5E2C9}">
   <dimension ref="A1:B37"/>
   <sheetViews>
@@ -2133,7 +2570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB852AE-A4C7-4284-9FBD-1CEEB9311916}">
   <dimension ref="A1:B18"/>
   <sheetViews>
@@ -2297,12 +2734,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CD6236-1D5E-43C4-8447-268AAEF1A0C5}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2495,7 +2932,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF4F714-5A64-4B0A-90E7-28D299FDF6BE}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -2571,12 +3008,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AECD6F-4371-4391-B58E-E510CF964736}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2604,6 +3041,9 @@
       <c r="B2" s="7" t="s">
         <v>203</v>
       </c>
+      <c r="C2" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -2612,6 +3052,9 @@
       <c r="B3" s="7" t="s">
         <v>204</v>
       </c>
+      <c r="C3" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -2620,6 +3063,9 @@
       <c r="B4" s="7" t="s">
         <v>205</v>
       </c>
+      <c r="C4" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -2628,6 +3074,9 @@
       <c r="B5" s="7" t="s">
         <v>206</v>
       </c>
+      <c r="C5" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -2636,6 +3085,9 @@
       <c r="B6" s="7" t="s">
         <v>139</v>
       </c>
+      <c r="C6" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -2644,6 +3096,9 @@
       <c r="B7" s="7" t="s">
         <v>211</v>
       </c>
+      <c r="C7" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -2652,6 +3107,9 @@
       <c r="B8" s="7" t="s">
         <v>207</v>
       </c>
+      <c r="C8" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -2660,6 +3118,9 @@
       <c r="B9" s="7" t="s">
         <v>208</v>
       </c>
+      <c r="C9" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -2668,6 +3129,9 @@
       <c r="B10" s="7" t="s">
         <v>209</v>
       </c>
+      <c r="C10" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -2676,6 +3140,9 @@
       <c r="B11" s="7" t="s">
         <v>210</v>
       </c>
+      <c r="C11" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -2684,6 +3151,9 @@
       <c r="B12" s="7" t="s">
         <v>212</v>
       </c>
+      <c r="C12" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -2692,6 +3162,9 @@
       <c r="B13" s="7" t="s">
         <v>216</v>
       </c>
+      <c r="C13" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -2734,92 +3207,6 @@
         <v>227</v>
       </c>
       <c r="C17" t="s">
-        <v>222</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD4CE82-100F-475B-B66F-A9CBAA32385B}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="83.21875" customWidth="1"/>
-    <col min="2" max="2" width="47.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="C2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="C3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="C4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="C5" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="C6" t="s">
         <v>222</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated parser to take in metadata
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1343685E-83EA-4503-8F9D-DA3A2F421BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5392D5-FB20-4E82-BCBA-9FBD53E19C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basis For Selection" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="305">
   <si>
     <t>Answer</t>
   </si>
@@ -925,25 +925,31 @@
     <t>Template</t>
   </si>
   <si>
-    <t>Operation Allowed?</t>
-  </si>
-  <si>
-    <t>Sum up?</t>
-  </si>
-  <si>
-    <t>Answer Range?</t>
-  </si>
-  <si>
-    <t>Percentage</t>
-  </si>
-  <si>
     <t>About</t>
   </si>
   <si>
-    <t xml:space="preserve">The {aggregation} of students {range} in the {initial_final} {year} cohort {} is {value} </t>
-  </si>
-  <si>
     <t>For student cohort data, you can ask about students exemptions from a cohort year, number of students who graduated within four, five, or six year and graduation rate for those years. You can also ask all of the things paired with financial aid in terms of student who received pell-grant, student who received stafford loan but not pell grant and student who received neither.</t>
+  </si>
+  <si>
+    <t>Operation-Allowed?</t>
+  </si>
+  <si>
+    <t>Sum-Allowed?</t>
+  </si>
+  <si>
+    <t>Range-Alllowed?</t>
+  </si>
+  <si>
+    <t>The $aggregation of students {who graduated $range $number years and $range $number years} in the $initial_final $year cohort is [value]</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Percentage-Allowed?</t>
+  </si>
+  <si>
+    <t>Metadata</t>
   </si>
 </sst>
 </file>
@@ -1292,7 +1298,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1555,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7606B2B-8397-4A8E-AF38-C293D77D8867}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="104" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1719,33 +1725,33 @@
         <v>294</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B22" s="6" t="s">
         <v>301</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>222</v>
@@ -1753,7 +1759,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>222</v>
@@ -1761,9 +1767,17 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>222</v>
       </c>
     </row>
@@ -2423,8 +2437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20057133-7837-4203-86B9-F46D32350538}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2595,7 +2609,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added enrollment questions, fixed discrete range logic, taking into account sparse matrix metadata when finding answers. Next step trying to get test cases to pass
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5392D5-FB20-4E82-BCBA-9FBD53E19C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351D02C3-B320-47F8-AC01-7F9058AF6FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Basis For Selection" sheetId="1" r:id="rId1"/>
-    <sheet name="Cohort" sheetId="10" r:id="rId2"/>
-    <sheet name="Admission Policies" sheetId="9" r:id="rId3"/>
-    <sheet name="Freshman Profile_Percentile" sheetId="2" r:id="rId4"/>
-    <sheet name="Freshman Profile_SAT Score " sheetId="3" r:id="rId5"/>
-    <sheet name="Freshman Profile_SAT Score" sheetId="11" r:id="rId6"/>
-    <sheet name="Freshman Profile_Class Rank GPA" sheetId="4" r:id="rId7"/>
-    <sheet name="Transfer Admission_General" sheetId="5" r:id="rId8"/>
-    <sheet name="Student Life_Categories" sheetId="7" r:id="rId9"/>
-    <sheet name="Student Life_Offered" sheetId="8" r:id="rId10"/>
+    <sheet name="Enrollment_General" sheetId="12" r:id="rId1"/>
+    <sheet name="Enrollment_Race" sheetId="13" r:id="rId2"/>
+    <sheet name="Basis For Selection" sheetId="1" r:id="rId3"/>
+    <sheet name="Cohort" sheetId="10" r:id="rId4"/>
+    <sheet name="Admission Policies" sheetId="9" r:id="rId5"/>
+    <sheet name="Freshman Profile_Percentile" sheetId="2" r:id="rId6"/>
+    <sheet name="Freshman Profile_SAT Score " sheetId="3" r:id="rId7"/>
+    <sheet name="Freshman Profile_SAT Score" sheetId="11" r:id="rId8"/>
+    <sheet name="Freshman Profile_Class Rank GPA" sheetId="4" r:id="rId9"/>
+    <sheet name="Transfer Admission_General" sheetId="5" r:id="rId10"/>
+    <sheet name="Student Life_Categories" sheetId="7" r:id="rId11"/>
+    <sheet name="Student Life_Offered" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="361">
   <si>
     <t>Answer</t>
   </si>
@@ -937,9 +939,6 @@
     <t>Sum-Allowed?</t>
   </si>
   <si>
-    <t>Range-Alllowed?</t>
-  </si>
-  <si>
     <t>The $aggregation of students {who graduated $range $number years and $range $number years} in the $initial_final $year cohort is [value]</t>
   </si>
   <si>
@@ -950,6 +949,177 @@
   </si>
   <si>
     <t>Metadata</t>
+  </si>
+  <si>
+    <t>Range-Allowed?</t>
+  </si>
+  <si>
+    <t>Basis of selection is about the importance of different factors in admission decisions. For basis of selection you can ask about the importance of the following for admission decisions: rigor of secondary school records, class rank, gpa, standardized test scores, recommendation letter, interview, extracirricular activities, talent/ability, character/personal qualities, first generation student, alumni relation, geographic residence, religious affiliation/commitment, racial/ethnic status, volunteer work, work experience, level of applicant's interest.</t>
+  </si>
+  <si>
+    <t>How many male full-time undergraduate degree-seeking first-time freshmen are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female full-time undergraduate degree-seeking first-time freshmen are enrolled?</t>
+  </si>
+  <si>
+    <t>How many male part-time undergraduate degree-seeking first-time freshmen are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female part-time undergraduate degree-seeking first-time freshmen are enrolled?</t>
+  </si>
+  <si>
+    <t>How many male full-time undergraduate non-first-time-freshman first-year students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female full-time undergraduate non-first-time-freshman first-year students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many male part-time undergraduate non-first-time-freshman first-year students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female part-time undergraduate non-first-time-freshman first-year students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many male full-time undergraduate degree-seeking non-freshmen are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female full-time undergraduate degree-seeking non-freshmen are enrolled?</t>
+  </si>
+  <si>
+    <t>How many male part-time undergraduate degree-seeking non-freshmen are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female part-time undergraduate degree-seeking non-freshmen are enrolled?</t>
+  </si>
+  <si>
+    <t>How many male full-time undergraduate degree-seeking students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female full-time undergraduate degree-seeking students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many male part-time undergraduate degree-seeking students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female part-time undergraduate degree-seeking students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many male full-time undergraduate non-degree-seeking students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female full-time undergraduate non-degree-seeking students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many male part-time undergraduate non-degree-seeking students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female part-time undergraduate non-degree-seeking students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many male full-time graduate degree-seeking first-time students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female full-time graduate degree-seeking first-time students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many male part-time graduate degree-seeking first-time students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female part-time graduate degree-seeking first-time students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many male full-time graduate degree-seeking non-first-time students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female full-time graduate degree-seeking non-first-time students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many male part-time graduate degree-seeking non-first-time students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female part-time graduate degree-seeking non-first-time students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many male full-time graduate non-degree-seeking students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female full-time graduate non-degree-seeking students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many male part-time graduate non-degree-seeking students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many female part-time graduate non-degree-seeking students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year nonresident aliens are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking undergraduate nonresident aliens are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year hispanics are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking undergraduate hispanics are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year african americans are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking undergraduate african americans are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year white students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking undergraduate white students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year american indians are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking undergraduate american indians are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year asians are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking undergraduate asians are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year pacific islanders are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking undergraduate pacific islanders are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year students of two or more races are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking undergraduate students of two or more races are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year students of unknown race are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking undergraduate students of unknown race are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year students are enrolled?</t>
+  </si>
+  <si>
+    <t>For student cohorts, you can ask about students exemptions from a cohort year, number of students who graduated within four, five, or six year and graduation rate for those years. You can also ask all of the things paired with financial aid in terms of student who received pell-grant, student who received stafford loan but not pell grant and student who received neither.</t>
+  </si>
+  <si>
+    <t>Denominator-Question</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>The [aggregation] of [gender] [is_first_time] [is_first_year] [undergraduate_grade_level] [degree-goal] [student_level] enrolled is &lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -1294,17 +1464,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F776689-DE3B-468A-9224-18F5400CC444}">
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="81.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="97.5546875" customWidth="1"/>
+    <col min="2" max="2" width="119.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1317,163 +1487,808 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>306</v>
+      </c>
+      <c r="B2">
+        <v>481</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>307</v>
+      </c>
+      <c r="B3">
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>308</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>309</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>310</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>311</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>312</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>313</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>314</v>
+      </c>
+      <c r="B10">
+        <v>1056</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>315</v>
+      </c>
+      <c r="B11">
+        <v>345</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>316</v>
+      </c>
+      <c r="B12">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>21</v>
+        <v>317</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>21</v>
+        <v>318</v>
+      </c>
+      <c r="B14">
+        <v>1551</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>319</v>
+      </c>
+      <c r="B15">
+        <v>503</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>320</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>321</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>322</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>323</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>21</v>
+        <v>324</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="B34" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B36" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B37" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B38" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B39" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B40" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="B55" s="7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B56" s="6" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" s="7" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CD6236-1D5E-43C4-8447-268AAEF1A0C5}">
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="131" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" s="7">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B24" s="7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" s="7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B27" s="7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AECD6F-4371-4391-B58E-E510CF964736}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="131.44140625" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C10" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C12" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C14" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C15" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C16" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD4CE82-100F-475B-B66F-A9CBAA32385B}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1560,11 +2375,437 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8ED044F-2B62-42B7-A288-F87892E20B00}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="83.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B5">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B7">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B8">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B9">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B12">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B13">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B17">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B19">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="B20" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B23" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B24" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B25" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B26" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B27" t="s">
+        <v>356</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" zoomScale="82" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="81.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="388.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7606B2B-8397-4A8E-AF38-C293D77D8867}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1727,10 +2968,10 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -1738,7 +2979,7 @@
         <v>296</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1746,7 +2987,7 @@
         <v>295</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -1767,7 +3008,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>222</v>
@@ -1775,7 +3016,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>222</v>
@@ -1787,7 +3028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0908D19-61E8-460E-9695-3943D19E115C}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -1938,7 +3179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3892E9F-E7EA-42B9-AE4C-1275BBD6A387}">
   <dimension ref="A1:C37"/>
   <sheetViews>
@@ -2258,7 +3499,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C307D05E-B833-4D75-9855-8E27A1B5E2C9}">
   <dimension ref="A1:B19"/>
   <sheetViews>
@@ -2433,7 +3674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20057133-7837-4203-86B9-F46D32350538}">
   <dimension ref="A1:B19"/>
   <sheetViews>
@@ -2604,7 +3845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB852AE-A4C7-4284-9FBD-1CEEB9311916}">
   <dimension ref="A1:B18"/>
   <sheetViews>
@@ -2766,457 +4007,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CD6236-1D5E-43C4-8447-268AAEF1A0C5}">
-  <dimension ref="A1:C28"/>
-  <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="131" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59" style="7" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4" s="7">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B5" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="B6" s="7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="B7" s="7">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B8" s="7">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="B9" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B24" s="7">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B25" s="7">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B27" s="7">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AECD6F-4371-4391-B58E-E510CF964736}">
-  <dimension ref="A1:C17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="131.44140625" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="C2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="C3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="C4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="C5" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="C7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C8" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="C9" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="C10" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="C11" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C12" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="C13" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="C14" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="C15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="C16" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="C17" t="s">
-        <v>222</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
training data for financial aid
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF33833-3F13-4404-BD5D-49D44CF587EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF57765-696A-4B3A-9AE3-D1BC33745C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="19" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enrollment_General" sheetId="12" r:id="rId1"/>
@@ -30,6 +30,10 @@
     <sheet name="Transfer Admission_Statistic" sheetId="17" r:id="rId15"/>
     <sheet name="Student Life_Categories" sheetId="7" r:id="rId16"/>
     <sheet name="Student Life_Offered" sheetId="8" r:id="rId17"/>
+    <sheet name="Financial Aid_Awarded" sheetId="19" r:id="rId18"/>
+    <sheet name="Financial Aid_Awarded Freshman" sheetId="20" r:id="rId19"/>
+    <sheet name="Financial Aid_Awarded Undergrad" sheetId="21" r:id="rId20"/>
+    <sheet name="Financial Aid_Awarded Part-Time" sheetId="22" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="464">
   <si>
     <t>Answer</t>
   </si>
@@ -1099,9 +1103,6 @@
     <t>Denominator-Question</t>
   </si>
   <si>
-    <t>The [aggregation] of [gender] [is_first_time] [is_first_year] [undergraduate_grade_level] [degree-goal] [student_level] enrolled is &lt;value&gt;</t>
-  </si>
-  <si>
     <t>The [aggregation][ of students {who graduated in [range] [number] years and [range] [number] years} in the [initial_final] [year] cohort is [value]</t>
   </si>
   <si>
@@ -1127,6 +1128,327 @@
   </si>
   <si>
     <t>1.0%</t>
+  </si>
+  <si>
+    <t>The [aggregation] of [gender] [is_first_time] [is_first_year] [undergraduate_grade_level] [degree-goal] [student_level] students enrolled is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>Which needs-analysis methodology does your institution use in awarding institutional aid?</t>
+  </si>
+  <si>
+    <t>What is the amount of need-based federal scholarship or grants awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of non-need-based federal scholarship or grants awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of need-based state scholarship or grants awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of non-need-based state scholarship or grants awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of need-based institutional scholarship or grants awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of non-need-based institutional scholarship or grants awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of need-based scholarship or grants from external sources awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of non-need-based scholarship or grants from external sources awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of need-based student loan awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of non-need-based student loan awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of need-based federal work study awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of need-based state and other work study awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the total amount of need-based self-help awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the total amount of non-need-based self-help awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of need-based parent loans awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of non-need-based parent loans awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the number of full-time full-time freshman students who applied for need-based financial aid</t>
+  </si>
+  <si>
+    <t>What is the number of  degree-seeking first-time full-time freshman students that applied for need-based financial aid and were determined to have financial need</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking first-time full-time freshman students who were determined to have financial need and were awarded any financial aid.</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking first-time full-time freshman students who were awarded any need-based scholarship or grant aid?</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking first-time full-time freshman students who were awarded any need-based self-help aid</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking first-time full-time freshman students who were awarded any non-need-based scholarship or grant aid</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking first-time full-time freshman students whose financial need was fully met </t>
+  </si>
+  <si>
+    <t>On average, what is the percentage of financial need that was met for degree-seeking first-time full-time freshman students who were awarded any need-based aid?</t>
+  </si>
+  <si>
+    <t>What is the average financial aid package for degree-seeking first-time full-time freshman students who were awarded any financial aid?</t>
+  </si>
+  <si>
+    <t>What is the average need-based scholarship or grant awarded to degree-seeking first-time full-time freshman students?</t>
+  </si>
+  <si>
+    <t>What is the average need-based self-help awarded to degree-seeking first-time full-time freshman students ?</t>
+  </si>
+  <si>
+    <t>What is the average need-based loan of students who were awarded any need-based self-help aid?</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking first-time full-time freshman students who had no financial need and who were awarded institutional non-need-based scholarship or grant aid?</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking first-time full-time freshman students who were awarded an institutional non-need-based athletic scholarship or grant?</t>
+  </si>
+  <si>
+    <t>What is the average amount of institutional non-need-based athletic scholarship and grant to degree-seeking first-time full-time freshman students?</t>
+  </si>
+  <si>
+    <t>What is the average amount of institutional non-need-based scholarship and grant aid awarded to degree-seeking full-time freshman students who had no financial need and who were awarded institutional non-need-based scholarship or grant aid?</t>
+  </si>
+  <si>
+    <t>What is the average need-based loan of degree-seeking first-time full-time freshman  students who were awarded any need-based self-help aid?</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking full-time undergraduate students who applied for need-based financial aid</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking full-time undergraduate students that applied for need-based financial aid and were determined to have financial need</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking full-time undergraduate students who were determined to have financial need and were awarded any financial aid.</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking full-time undergraduate students who were awarded any need-based scholarship or grant aid?</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking full-time undergraduate students who were awarded any need-based self-help aid</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking full-time undergraduate students who were awarded any non-need-based scholarship or grant aid</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking full-time undergraduate students whose financial need was fully met </t>
+  </si>
+  <si>
+    <t>On average, what is the percentage of financial need that was met for degree-seeking full-time undergraduate students who were awarded any need-based aid?</t>
+  </si>
+  <si>
+    <t>What is the average financial aid package for degree-seeking full-time undergraduate students who were awarded any financial aid?</t>
+  </si>
+  <si>
+    <t>What is the average need-based scholarship or grant awarded to degree-seeking full-time undergraduate students?</t>
+  </si>
+  <si>
+    <t>What is the average need-based self-help awarded to degree-seeking full-time undergraduate students ?</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking full-time undergraduate students who had no financial need and who were awarded institutional non-need-based scholarship or grant aid?</t>
+  </si>
+  <si>
+    <t>What is the average amount of institutional non-need-based scholarship and grant aid award to degree-seeking full-time students who had no financial need and who were awarded institutional non-need-based scholarship or grant aid?</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking full-time undergraduate students who were awarded an institutional non-need-based athletic scholarship or grant?</t>
+  </si>
+  <si>
+    <t>What is the average amount of institutional non-need-based athletic scholarship and grant to degree-seeking full-time undergraduate students?</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking part-time undergraduate students who applied for need-based financial aid</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking part-time undergraduate students that applied for need-based financial aid and were determined to have financial need</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking part-time undergraduate students who were determined to have financial need and were awarded any financial aid.</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking part-time undergraduate students who were awarded any need-based scholarship or grant aid?</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking part-time undergraduate students who were awarded any need-based self-help aid</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking part-time undergraduate students who were awarded any non-need-based scholarship or grant aid</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking part-time undergraduate students whose financial need was fully met </t>
+  </si>
+  <si>
+    <t>On average, what is the percentage of financial need that was met for degree-seeking part-time undergraduate students who were awarded any need-based aid?</t>
+  </si>
+  <si>
+    <t>What is the average financial aid package for degree-seeking part-time undergraduate students who were awarded any financial aid?</t>
+  </si>
+  <si>
+    <t>What is the average need-based scholarship or grant awarded to degree-seeking part-time undergraduate students?</t>
+  </si>
+  <si>
+    <t>What is the average need-based self-help awarded to degree-seeking part-time undergraduate students ?</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking part-time undergraduate students who had no financial need and who were awarded institutional non-need-based scholarship or grant aid?</t>
+  </si>
+  <si>
+    <t>What is the average amount of institutional non-need-based scholarship and grant aid award to degree-seeking part-time students who had no financial need and who were awarded institutional non-need-based scholarship or grant aid?</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking part-time undergraduate students who were awarded an institutional non-need-based athletic scholarship or grant?</t>
+  </si>
+  <si>
+    <t>What is the average amount of institutional non-need-based athletic scholarship and grant to degree-seeking part-time undergraduate students?</t>
+  </si>
+  <si>
+    <t>$1355304</t>
+  </si>
+  <si>
+    <t>$0</t>
+  </si>
+  <si>
+    <t>$856068</t>
+  </si>
+  <si>
+    <t>$8748</t>
+  </si>
+  <si>
+    <t>$34630806</t>
+  </si>
+  <si>
+    <t>$13098841</t>
+  </si>
+  <si>
+    <t>$738685</t>
+  </si>
+  <si>
+    <t>$10691241</t>
+  </si>
+  <si>
+    <t>$979015</t>
+  </si>
+  <si>
+    <t>$771042</t>
+  </si>
+  <si>
+    <t>What is the amount of non-need-based federal work study awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of non-need-based state and other work study awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of need-based tuition waiver aid awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of non-need-based tuition waiver aid awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of need-based athletic award awarded to students?</t>
+  </si>
+  <si>
+    <t>What is the amount of non-based athletic award awarded to students?</t>
+  </si>
+  <si>
+    <t>$11462283</t>
+  </si>
+  <si>
+    <t>$4938549</t>
+  </si>
+  <si>
+    <t>$375919</t>
+  </si>
+  <si>
+    <t>Rose-Hulman uses federal methology in awarding institutional aid.</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>73.5%</t>
+  </si>
+  <si>
+    <t>$39903</t>
+  </si>
+  <si>
+    <t>$38185</t>
+  </si>
+  <si>
+    <t>$3840</t>
+  </si>
+  <si>
+    <t>$3327</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>$21671</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>1394</t>
+  </si>
+  <si>
+    <t>$35451</t>
+  </si>
+  <si>
+    <t>$33608</t>
+  </si>
+  <si>
+    <t>$4679</t>
+  </si>
+  <si>
+    <t>$4351</t>
+  </si>
+  <si>
+    <t>794</t>
+  </si>
+  <si>
+    <t>$16643</t>
+  </si>
+  <si>
+    <t>64.7%</t>
+  </si>
+  <si>
+    <t>$26732</t>
+  </si>
+  <si>
+    <t>$24932</t>
+  </si>
+  <si>
+    <t>$4500</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>$14293</t>
   </si>
 </sst>
 </file>
@@ -1174,7 +1496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1191,6 +1513,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1474,14 +1802,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F776689-DE3B-468A-9224-18F5400CC444}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="97.5546875" customWidth="1"/>
-    <col min="2" max="2" width="29.77734375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="66.109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1729,12 +2057,12 @@
         <v>291</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>290</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1967,7 +2295,7 @@
         <v>93</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2081,7 +2409,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2392,7 +2720,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2518,7 +2846,7 @@
         <v>165</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C13" t="s">
         <v>220</v>
@@ -2573,7 +2901,7 @@
         <v>188</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C18" t="s">
         <v>220</v>
@@ -2584,7 +2912,7 @@
         <v>189</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C19" t="s">
         <v>220</v>
@@ -2606,7 +2934,7 @@
         <v>171</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C21" t="s">
         <v>220</v>
@@ -2804,7 +3132,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2822,7 +3150,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3057,7 +3385,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3075,7 +3403,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
@@ -3177,6 +3505,419 @@
       </c>
       <c r="B12" t="s">
         <v>258</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E00C0EE-B5EA-4C5D-A3F6-0409760A68CF}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="78.77734375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B25" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="B26"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B27" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B28" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B29" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD85EB1-BDB8-4AEB-99D1-57DF875DFEB5}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="99.33203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2" s="7">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="B3" s="7">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B4" s="7">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B5" s="7">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B6" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="B7" s="7">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="B8" s="7">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -3334,6 +4075,316 @@
       </c>
       <c r="B18" t="s">
         <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE4F375-28FB-4634-A90F-E29F4CD5ADA1}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="85.88671875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="49.33203125" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="B6" s="5">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="B8" s="5">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>450</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EA6128-27F4-4911-A1F0-865B26420EEF}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="78.88671875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="40.33203125" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="B2" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="B3" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="B7" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>419</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -3555,7 +4606,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>266</v>
@@ -3686,7 +4737,7 @@
         <v>290</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -3944,7 +4995,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -4158,7 +5209,7 @@
         <v>37</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -4254,7 +5305,7 @@
         <v>62</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -4286,7 +5337,7 @@
         <v>33</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -4318,7 +5369,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -4350,7 +5401,7 @@
         <v>50</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -4382,7 +5433,7 @@
         <v>63</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -4447,7 +5498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF2A7F2-CEC5-4907-876C-DED9EAEEDD17}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finished adding training data for almost all sections
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -8,32 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF57765-696A-4B3A-9AE3-D1BC33745C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30642D70-B98E-4390-A6D1-A18ACF30869F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="19" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="20" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Enrollment_General" sheetId="12" r:id="rId1"/>
-    <sheet name="Enrollment_Race Undergraduate" sheetId="16" r:id="rId2"/>
-    <sheet name="Enrollment_Race Freshman" sheetId="13" r:id="rId3"/>
-    <sheet name="Cohort" sheetId="10" r:id="rId4"/>
-    <sheet name="Basis For Selection" sheetId="1" r:id="rId5"/>
-    <sheet name="Admission Policies" sheetId="9" r:id="rId6"/>
-    <sheet name="Freshman Profile_Percentile" sheetId="2" r:id="rId7"/>
-    <sheet name="Freshman Profile_SAT Score Comp" sheetId="14" r:id="rId8"/>
-    <sheet name="Freshman Profile_SAT Score Sub " sheetId="3" r:id="rId9"/>
-    <sheet name="Freshman Profile_ACT score comp" sheetId="15" r:id="rId10"/>
-    <sheet name="Freshman Profile_ACT Score sub" sheetId="11" r:id="rId11"/>
-    <sheet name="Freshman Profile_GPA" sheetId="4" r:id="rId12"/>
-    <sheet name="Freshman Profile_Class Rank" sheetId="18" r:id="rId13"/>
-    <sheet name="Transfer Admission_General" sheetId="5" r:id="rId14"/>
-    <sheet name="Transfer Admission_Statistic" sheetId="17" r:id="rId15"/>
-    <sheet name="Student Life_Categories" sheetId="7" r:id="rId16"/>
-    <sheet name="Student Life_Offered" sheetId="8" r:id="rId17"/>
-    <sheet name="Financial Aid_Awarded" sheetId="19" r:id="rId18"/>
-    <sheet name="Financial Aid_Awarded Freshman" sheetId="20" r:id="rId19"/>
-    <sheet name="Financial Aid_Awarded Undergrad" sheetId="21" r:id="rId20"/>
-    <sheet name="Financial Aid_Awarded Part-Time" sheetId="22" r:id="rId21"/>
+    <sheet name="General Info" sheetId="23" r:id="rId1"/>
+    <sheet name="Enrollment_General" sheetId="12" r:id="rId2"/>
+    <sheet name="Enrollment_Race Undergraduate" sheetId="16" r:id="rId3"/>
+    <sheet name="Enrollment_Race Freshman" sheetId="13" r:id="rId4"/>
+    <sheet name="Cohort" sheetId="10" r:id="rId5"/>
+    <sheet name="Basis For Selection" sheetId="1" r:id="rId6"/>
+    <sheet name="Admission Policies" sheetId="9" r:id="rId7"/>
+    <sheet name="Freshman Profile_Percentile" sheetId="2" r:id="rId8"/>
+    <sheet name="Freshman Profile_SAT Score Comp" sheetId="14" r:id="rId9"/>
+    <sheet name="Freshman Profile_SAT Score Sub " sheetId="3" r:id="rId10"/>
+    <sheet name="Freshman Profile_ACT score comp" sheetId="15" r:id="rId11"/>
+    <sheet name="Freshman Profile_ACT Score sub" sheetId="11" r:id="rId12"/>
+    <sheet name="Freshman Profile_GPA" sheetId="4" r:id="rId13"/>
+    <sheet name="Freshman Profile_Class Rank" sheetId="18" r:id="rId14"/>
+    <sheet name="Transfer Admission_General" sheetId="5" r:id="rId15"/>
+    <sheet name="Transfer Admission_Statistic" sheetId="17" r:id="rId16"/>
+    <sheet name="Student Life_Categories" sheetId="7" r:id="rId17"/>
+    <sheet name="Student Life_Offered" sheetId="8" r:id="rId18"/>
+    <sheet name="Financial Aid_Awarded" sheetId="19" r:id="rId19"/>
+    <sheet name="Financial Aid_Awarded Freshman" sheetId="20" r:id="rId20"/>
+    <sheet name="Financial Aid_Awarded Undergrad" sheetId="21" r:id="rId21"/>
+    <sheet name="Financial Aid_Awarded Part-Time" sheetId="22" r:id="rId22"/>
+    <sheet name="Faculty And Class Size_Gender" sheetId="24" r:id="rId23"/>
+    <sheet name="Faculty And Class Size_Degree" sheetId="25" r:id="rId24"/>
+    <sheet name="Faculty And Class Size_Other" sheetId="26" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="491">
   <si>
     <t>Answer</t>
   </si>
@@ -1449,6 +1453,87 @@
   </si>
   <si>
     <t>$14293</t>
+  </si>
+  <si>
+    <t>What is Rose-Hulman's mailing address?</t>
+  </si>
+  <si>
+    <t>What is Rose-Hulman admissions phone number?</t>
+  </si>
+  <si>
+    <t>What is Rose-Hulman’s www home page address / website?</t>
+  </si>
+  <si>
+    <t>What is Rose-Hulman admissions toll free phone number?</t>
+  </si>
+  <si>
+    <t>What is Rose-Hulman admissions office mailing address?</t>
+  </si>
+  <si>
+    <t>What is Rose-Hulman’s admission fax number?</t>
+  </si>
+  <si>
+    <t>What is Rose-Hulman’s email?</t>
+  </si>
+  <si>
+    <t>What is the url for Rose-Hulman’s online application?</t>
+  </si>
+  <si>
+    <t>What is the source of institutional control for Rose-Hulman. Is the institution a private or public college?</t>
+  </si>
+  <si>
+    <t>Is Rose-Hulman a coeducational college, men’s college or women’s college?</t>
+  </si>
+  <si>
+    <t>What academic year calendar does Rose-Hulman use? Is it quarter, semester, trimester, continuous, 4-1-4, or does it differ by program?</t>
+  </si>
+  <si>
+    <t>What degrees are offered by Rose-Hulman?</t>
+  </si>
+  <si>
+    <t>What is the total number of full-time instructional faculty who are women?</t>
+  </si>
+  <si>
+    <t>What is the total number of part-time instructional faculty who are women?</t>
+  </si>
+  <si>
+    <t>What is the total number of full-time instructional faculty who are men?</t>
+  </si>
+  <si>
+    <t>What is the total number of part-time instructional faculty who are men?</t>
+  </si>
+  <si>
+    <t>What is the total number of full-time instructional faculty who have a doctorate degree?</t>
+  </si>
+  <si>
+    <t>What is the total number of part-time instructional faculty who have a doctorate degree?</t>
+  </si>
+  <si>
+    <t>What is the total number of full-time instructional faculty whose highest degree is a masters </t>
+  </si>
+  <si>
+    <t>What is the total number of part-time instructional faculty whose highest degree is a masters</t>
+  </si>
+  <si>
+    <t>What is the total number of full-time instructional faculty whose highest degree is a bachelors </t>
+  </si>
+  <si>
+    <t>What is the total number of part-time instructional faculty whose highest degree is a bachelor</t>
+  </si>
+  <si>
+    <t>What is the total number of full-time instructional faculty whose highest degree is unknown</t>
+  </si>
+  <si>
+    <t>What is the total number of part-time instructional faculty whose highest degree is unknown</t>
+  </si>
+  <si>
+    <t>What is the total number of full-time instructional faculty in stand-alone graduate/professional programs in which instructional faculty teach virtually only graduate level students</t>
+  </si>
+  <si>
+    <t>What is the total number of part-time instructional faculty in stand-alone graduate/professional programs in which instructional faculty teach virtually only graduate level students</t>
+  </si>
+  <si>
+    <t>What is the student to faculty ratio at Rose-Hulman?</t>
   </si>
 </sst>
 </file>
@@ -1799,311 +1884,312 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F776689-DE3B-468A-9224-18F5400CC444}">
-  <dimension ref="A1:B36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E422E2F-D9FA-411F-968E-DE340F994DF5}">
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="97.5546875" customWidth="1"/>
-    <col min="2" max="2" width="66.109375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="78.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="C2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="C3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="C4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="C5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="C6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="C7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="C8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="C9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="C10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="C11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="C12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="C13" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C307D05E-B833-4D75-9855-8E27A1B5E2C9}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="114.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="B2" s="6">
-        <v>387</v>
+        <v>71</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="B3" s="6">
-        <v>143</v>
+        <v>72</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="B4" s="6">
-        <v>1</v>
+        <v>73</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0</v>
+        <v>74</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B6" s="6">
-        <v>9</v>
+        <v>75</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="B7" s="6">
-        <v>2</v>
+        <v>76</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="B8" s="6">
-        <v>0</v>
+        <v>77</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B9" s="6">
-        <v>0</v>
+        <v>78</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="B10" s="6">
-        <v>1082</v>
+        <v>69</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="B11" s="6">
-        <v>329</v>
+        <v>70</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B12" s="6">
-        <v>15</v>
+        <v>67</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="B13" s="6">
-        <v>1</v>
+        <v>68</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B14" s="6">
-        <v>0</v>
+      <c r="A14" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B14" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="B15" s="6">
-        <v>0</v>
-      </c>
+      <c r="A15" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="B15"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="B16" s="6">
-        <v>2</v>
-      </c>
+      <c r="A16" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B16"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="B17" s="6">
-        <v>1</v>
+      <c r="A17" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B17" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B18" s="6">
-        <v>3</v>
+      <c r="A18" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B18" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="B19" s="6">
-        <v>0</v>
+      <c r="A19" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B19" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="B20" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="B21" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="B22" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="B23" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="B24" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="B25" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="B26" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="B27" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="B28" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="B29" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+      <c r="A20" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B20" t="s">
         <v>258</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="B8" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3682DD5-C270-454D-A655-BE30A9BBE78A}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -2228,7 +2314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20057133-7837-4203-86B9-F46D32350538}">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -2404,7 +2490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB852AE-A4C7-4284-9FBD-1CEEB9311916}">
   <dimension ref="A1:B19"/>
   <sheetViews>
@@ -2572,7 +2658,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBBFCBD-BE53-4EBE-BC28-AF1024B4BD2D}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -2697,7 +2783,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CD6236-1D5E-43C4-8447-268AAEF1A0C5}">
   <dimension ref="A1:C28"/>
   <sheetViews>
@@ -3002,7 +3088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869E4568-D908-477D-923D-F4116B90EDC7}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -3127,7 +3213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AECD6F-4371-4391-B58E-E510CF964736}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -3380,7 +3466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD4CE82-100F-475B-B66F-A9CBAA32385B}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -3512,12 +3598,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E00C0EE-B5EA-4C5D-A3F6-0409760A68CF}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3737,7 +3823,7 @@
         <v>292</v>
       </c>
       <c r="B27" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -3770,7 +3856,312 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F776689-DE3B-468A-9224-18F5400CC444}">
+  <dimension ref="A1:B36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="97.5546875" customWidth="1"/>
+    <col min="2" max="2" width="66.109375" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2" s="6">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B3" s="6">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B6" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B11" s="6">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B12" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B16" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B18" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B20" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B22" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B23" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B24" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B28" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B29" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>258</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD85EB1-BDB8-4AEB-99D1-57DF875DFEB5}">
   <dimension ref="A1:B17"/>
   <sheetViews>
@@ -3925,7 +4316,477 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE4F375-28FB-4634-A90F-E29F4CD5ADA1}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="85.88671875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="49.33203125" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="B6" s="5">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="B8" s="5">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>450</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EA6128-27F4-4911-A1F0-865B26420EEF}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="78.88671875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="40.33203125" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="B2" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="B3" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="B7" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>419</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>450</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2A9967-94EA-41CF-ACB5-C81483AD239D}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="84.109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="36.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>479</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2758D6-F888-4498-88A0-7DFBF7091CA2}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="53.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>487</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ED34DA-E2CB-4859-9A96-48DF7AE0B7A7}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="36.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>490</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354727B8-DF4A-4CB3-BBB4-023F92A30B71}">
   <dimension ref="A1:B18"/>
   <sheetViews>
@@ -4082,317 +4943,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE4F375-28FB-4634-A90F-E29F4CD5ADA1}">
-  <dimension ref="A1:B17"/>
-  <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="85.88671875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="49.33203125" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="B6" s="5">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>398</v>
-      </c>
-      <c r="B8" s="5">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>404</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>450</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EA6128-27F4-4911-A1F0-865B26420EEF}">
-  <dimension ref="A1:B17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="78.88671875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="40.33203125" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="B2" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>408</v>
-      </c>
-      <c r="B3" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>410</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>411</v>
-      </c>
-      <c r="B6" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>412</v>
-      </c>
-      <c r="B7" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>414</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>415</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>416</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>417</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>418</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>419</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>420</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>421</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>450</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8ED044F-2B62-42B7-A288-F87892E20B00}">
   <dimension ref="A1:B18"/>
   <sheetViews>
@@ -4550,12 +5101,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7606B2B-8397-4A8E-AF38-C293D77D8867}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4778,7 +5329,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
@@ -4974,7 +5525,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0908D19-61E8-460E-9695-3943D19E115C}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -5125,7 +5676,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3892E9F-E7EA-42B9-AE4C-1275BBD6A387}">
   <dimension ref="A1:B44"/>
   <sheetViews>
@@ -5494,7 +6045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF2A7F2-CEC5-4907-876C-DED9EAEEDD17}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -5617,183 +6168,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C307D05E-B833-4D75-9855-8E27A1B5E2C9}">
-  <dimension ref="A1:B20"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="114.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="B14" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="B15"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="B16"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="B17" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="B18" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="B19" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="B20" t="s">
-        <v>258</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="B8" numberStoredAsText="1"/>
-  </ignoredErrors>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
full sentence using template, still need to test it out more
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30642D70-B98E-4390-A6D1-A18ACF30869F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5A26E8-214B-4B05-A02C-6FC79277F855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="20" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -1107,9 +1107,6 @@
     <t>Denominator-Question</t>
   </si>
   <si>
-    <t>The [aggregation][ of students {who graduated in [range] [number] years and [range] [number] years} in the [initial_final] [year] cohort is [value]</t>
-  </si>
-  <si>
     <t>How many of exempted students were recipients of a Subsidized Stafford Loan but not did not receive a Pell Grant?</t>
   </si>
   <si>
@@ -1534,6 +1531,9 @@
   </si>
   <si>
     <t>What is the student to faculty ratio at Rose-Hulman?</t>
+  </si>
+  <si>
+    <t>The [aggregation][ of students {who graduated in [range] [number] years and [range] [number] years} in the [initial_final] [year] cohort is &lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -1887,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E422E2F-D9FA-411F-968E-DE340F994DF5}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1906,12 +1906,12 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C2" t="s">
         <v>220</v>
@@ -1919,7 +1919,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C3" t="s">
         <v>220</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C4" t="s">
         <v>220</v>
@@ -1935,7 +1935,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C5" t="s">
         <v>220</v>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C6" t="s">
         <v>220</v>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C7" t="s">
         <v>220</v>
@@ -1959,7 +1959,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C8" t="s">
         <v>220</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C9" t="s">
         <v>220</v>
@@ -1975,7 +1975,7 @@
     </row>
     <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C10" t="s">
         <v>220</v>
@@ -1983,7 +1983,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C11" t="s">
         <v>220</v>
@@ -1991,7 +1991,7 @@
     </row>
     <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C12" t="s">
         <v>220</v>
@@ -1999,7 +1999,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C13" t="s">
         <v>220</v>
@@ -2381,7 +2381,7 @@
         <v>93</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2806,7 +2806,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2932,7 +2932,7 @@
         <v>165</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C13" t="s">
         <v>220</v>
@@ -2987,7 +2987,7 @@
         <v>188</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C18" t="s">
         <v>220</v>
@@ -2998,7 +2998,7 @@
         <v>189</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C19" t="s">
         <v>220</v>
@@ -3020,7 +3020,7 @@
         <v>171</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C21" t="s">
         <v>220</v>
@@ -3236,7 +3236,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3489,7 +3489,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
@@ -3622,186 +3622,186 @@
     </row>
     <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -3860,8 +3860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F776689-DE3B-468A-9224-18F5400CC444}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4120,7 +4120,7 @@
         <v>290</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -4185,7 +4185,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B2" s="7">
         <v>466</v>
@@ -4193,7 +4193,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B3" s="7">
         <v>360</v>
@@ -4201,7 +4201,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B4" s="7">
         <v>360</v>
@@ -4209,7 +4209,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B5" s="7">
         <v>357</v>
@@ -4217,7 +4217,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B6" s="7">
         <v>236</v>
@@ -4225,7 +4225,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B7" s="7">
         <v>168</v>
@@ -4233,7 +4233,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B8" s="7">
         <v>124</v>
@@ -4241,74 +4241,74 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -4340,15 +4340,15 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B3" s="5">
         <v>1151</v>
@@ -4356,7 +4356,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B4" s="5">
         <v>1150</v>
@@ -4364,7 +4364,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B5" s="5">
         <v>1144</v>
@@ -4372,7 +4372,7 @@
     </row>
     <row r="6" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B6" s="5">
         <v>829</v>
@@ -4380,7 +4380,7 @@
     </row>
     <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B7" s="5">
         <v>1009</v>
@@ -4388,7 +4388,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B8" s="5">
         <v>284</v>
@@ -4396,7 +4396,7 @@
     </row>
     <row r="9" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>64</v>
@@ -4404,66 +4404,66 @@
     </row>
     <row r="10" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -4495,7 +4495,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B2" s="5">
         <v>6</v>
@@ -4503,7 +4503,7 @@
     </row>
     <row r="3" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B3" s="5">
         <v>5</v>
@@ -4511,7 +4511,7 @@
     </row>
     <row r="4" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>287</v>
@@ -4519,7 +4519,7 @@
     </row>
     <row r="5" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>287</v>
@@ -4527,7 +4527,7 @@
     </row>
     <row r="6" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B6" s="5">
         <v>2</v>
@@ -4535,7 +4535,7 @@
     </row>
     <row r="7" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B7" s="5">
         <v>5</v>
@@ -4543,7 +4543,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -4551,74 +4551,74 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -4650,22 +4650,22 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -4697,42 +4697,42 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -4744,7 +4744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ED34DA-E2CB-4859-9A96-48DF7AE0B7A7}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4763,22 +4763,22 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="69" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="69" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -4791,7 +4791,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5105,8 +5105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7606B2B-8397-4A8E-AF38-C293D77D8867}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5157,7 +5157,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>266</v>
@@ -5288,7 +5288,7 @@
         <v>290</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>348</v>
+        <v>490</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -5546,7 +5546,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -5681,7 +5681,7 @@
   <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="105" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5760,7 +5760,7 @@
         <v>37</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -5856,7 +5856,7 @@
         <v>62</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -5888,7 +5888,7 @@
         <v>33</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -5920,7 +5920,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -5952,7 +5952,7 @@
         <v>50</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -5984,7 +5984,7 @@
         <v>63</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fixed template converter and changed some entity
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624AE331-1895-4489-ABE9-BF5D66F099C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25E40D6-51F0-49E2-BD0F-8869454E856F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="493">
   <si>
     <t>Answer</t>
   </si>
@@ -1185,9 +1185,6 @@
     <t>What is the amount of non-need-based parent loans awarded to students?</t>
   </si>
   <si>
-    <t>What is the number of full-time full-time freshman students who applied for need-based financial aid</t>
-  </si>
-  <si>
     <t>What is the number of  degree-seeking first-time full-time freshman students that applied for need-based financial aid and were determined to have financial need</t>
   </si>
   <si>
@@ -1534,6 +1531,15 @@
   </si>
   <si>
     <t>The (or [aggregation] number) of students {who graduated in [range] [number] years and [range] [number] years} in the [initial_final] [year] cohort is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking full-time full-time freshman students who applied for need-based financial aid</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (xor { on [aggregation], the [aggregation] } {The number}) of degree-seeking, first-time, full-time freshman students (xor {whose need was [financial_aid_degree_met] } {who were awarded any [need_non_need_base_aid] (xor [financial_aid_type]  institutional) (xor  [self-help] scholarship and grant) }) aid</t>
+  </si>
+  <si>
+    <t>The (xor [percentile] [aggregation]) score for [standarized_test] [subject] is &lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -1887,8 +1893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E422E2F-D9FA-411F-968E-DE340F994DF5}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1911,7 +1917,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C2" t="s">
         <v>220</v>
@@ -1919,7 +1925,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C3" t="s">
         <v>220</v>
@@ -1927,7 +1933,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C4" t="s">
         <v>220</v>
@@ -1935,7 +1941,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C5" t="s">
         <v>220</v>
@@ -1943,7 +1949,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C6" t="s">
         <v>220</v>
@@ -1951,7 +1957,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C7" t="s">
         <v>220</v>
@@ -1959,7 +1965,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C8" t="s">
         <v>220</v>
@@ -1967,7 +1973,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C9" t="s">
         <v>220</v>
@@ -1975,7 +1981,7 @@
     </row>
     <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C10" t="s">
         <v>220</v>
@@ -1983,7 +1989,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C11" t="s">
         <v>220</v>
@@ -1991,7 +1997,7 @@
     </row>
     <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C12" t="s">
         <v>220</v>
@@ -1999,7 +2005,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C13" t="s">
         <v>220</v>
@@ -2015,7 +2021,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2495,7 +2501,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2663,7 +2669,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2788,7 +2794,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3093,7 +3099,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A8" sqref="A8:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3218,7 +3224,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3471,7 +3477,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3602,8 +3608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E00C0EE-B5EA-4C5D-A3F6-0409760A68CF}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3625,7 +3631,7 @@
         <v>357</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3633,7 +3639,7 @@
         <v>358</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
@@ -3641,7 +3647,7 @@
         <v>359</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -3649,7 +3655,7 @@
         <v>360</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
@@ -3657,7 +3663,7 @@
         <v>361</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
@@ -3665,7 +3671,7 @@
         <v>362</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
@@ -3673,7 +3679,7 @@
         <v>363</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
@@ -3681,7 +3687,7 @@
         <v>364</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
@@ -3689,7 +3695,7 @@
         <v>365</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -3697,7 +3703,7 @@
         <v>366</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -3705,7 +3711,7 @@
         <v>367</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -3713,15 +3719,15 @@
         <v>368</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -3729,15 +3735,15 @@
         <v>369</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3745,7 +3751,7 @@
         <v>370</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -3753,7 +3759,7 @@
         <v>371</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -3761,7 +3767,7 @@
         <v>372</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -3769,39 +3775,39 @@
         <v>373</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -3861,7 +3867,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4163,16 +4169,16 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD85EB1-BDB8-4AEB-99D1-57DF875DFEB5}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="99.33203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="67.109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -4183,9 +4189,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>374</v>
+        <v>490</v>
       </c>
       <c r="B2" s="7">
         <v>466</v>
@@ -4193,7 +4199,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B3" s="7">
         <v>360</v>
@@ -4201,7 +4207,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B4" s="7">
         <v>360</v>
@@ -4209,7 +4215,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B5" s="7">
         <v>357</v>
@@ -4217,7 +4223,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B6" s="7">
         <v>236</v>
@@ -4225,7 +4231,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B7" s="7">
         <v>168</v>
@@ -4233,7 +4239,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B8" s="7">
         <v>124</v>
@@ -4241,74 +4247,127 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>449</v>
+        <v>448</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B18" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B21" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B22" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B23" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B24" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -4320,7 +4379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE4F375-28FB-4634-A90F-E29F4CD5ADA1}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -4340,15 +4399,15 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B3" s="5">
         <v>1151</v>
@@ -4356,7 +4415,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B4" s="5">
         <v>1150</v>
@@ -4364,7 +4423,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B5" s="5">
         <v>1144</v>
@@ -4372,7 +4431,7 @@
     </row>
     <row r="6" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B6" s="5">
         <v>829</v>
@@ -4380,7 +4439,7 @@
     </row>
     <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B7" s="5">
         <v>1009</v>
@@ -4388,7 +4447,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B8" s="5">
         <v>284</v>
@@ -4396,7 +4455,7 @@
     </row>
     <row r="9" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>64</v>
@@ -4404,66 +4463,66 @@
     </row>
     <row r="10" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -4475,8 +4534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EA6128-27F4-4911-A1F0-865B26420EEF}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4495,7 +4554,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B2" s="5">
         <v>6</v>
@@ -4503,7 +4562,7 @@
     </row>
     <row r="3" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B3" s="5">
         <v>5</v>
@@ -4511,7 +4570,7 @@
     </row>
     <row r="4" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>287</v>
@@ -4519,7 +4578,7 @@
     </row>
     <row r="5" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>287</v>
@@ -4527,7 +4586,7 @@
     </row>
     <row r="6" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B6" s="5">
         <v>2</v>
@@ -4535,7 +4594,7 @@
     </row>
     <row r="7" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B7" s="5">
         <v>5</v>
@@ -4543,7 +4602,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -4551,74 +4610,74 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -4631,7 +4690,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A16"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4650,22 +4709,22 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
   </sheetData>
@@ -4697,42 +4756,42 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -4768,17 +4827,17 @@
     </row>
     <row r="2" spans="1:3" ht="69" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="69" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
   </sheetData>
@@ -4948,7 +5007,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5105,7 +5164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7606B2B-8397-4A8E-AF38-C293D77D8867}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -5288,7 +5347,7 @@
         <v>290</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -5333,8 +5392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5530,7 +5589,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="58.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5680,14 +5739,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3892E9F-E7EA-42B9-AE4C-1275BBD6A387}">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="105" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="105" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="81.21875" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="67" style="5" customWidth="1"/>
     <col min="3" max="3" width="19.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6005,7 +6064,9 @@
       <c r="A40" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B40"/>
+      <c r="B40" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">

</xml_diff>

<commit_message>
rewrote parser to be asynchronous. Created api for parsing input data and frontend code for processing excel file
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\NewCDSDataFromClient\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\irpa_db\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0ADEF5-F9DA-4991-B94C-95CCC657018B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D6AA49-AF07-43BB-B6AA-5FE2CFDADF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -978,55 +978,28 @@
     <t>How many female part-time graduate non-degree-seeking students are enrolled?</t>
   </si>
   <si>
-    <t>How many degree-seeking first-time first-year nonresident aliens are enrolled?</t>
-  </si>
-  <si>
     <t>How many degree-seeking undergraduate nonresident aliens are enrolled?</t>
   </si>
   <si>
-    <t>How many degree-seeking first-time first-year hispanics are enrolled?</t>
-  </si>
-  <si>
     <t>How many degree-seeking undergraduate hispanics are enrolled?</t>
   </si>
   <si>
-    <t>How many degree-seeking first-time first-year african americans are enrolled?</t>
-  </si>
-  <si>
     <t>How many degree-seeking undergraduate african americans are enrolled?</t>
   </si>
   <si>
-    <t>How many degree-seeking first-time first-year white students are enrolled?</t>
-  </si>
-  <si>
     <t>How many degree-seeking undergraduate white students are enrolled?</t>
   </si>
   <si>
-    <t>How many degree-seeking first-time first-year american indians are enrolled?</t>
-  </si>
-  <si>
     <t>How many degree-seeking undergraduate american indians are enrolled?</t>
   </si>
   <si>
-    <t>How many degree-seeking first-time first-year asians are enrolled?</t>
-  </si>
-  <si>
     <t>How many degree-seeking undergraduate asians are enrolled?</t>
   </si>
   <si>
-    <t>How many degree-seeking first-time first-year pacific islanders are enrolled?</t>
-  </si>
-  <si>
     <t>How many degree-seeking undergraduate pacific islanders are enrolled?</t>
   </si>
   <si>
-    <t>How many degree-seeking first-time first-year students of two or more races are enrolled?</t>
-  </si>
-  <si>
     <t>How many degree-seeking undergraduate students of two or more races are enrolled?</t>
-  </si>
-  <si>
-    <t>How many degree-seeking first-time first-year students of unknown race are enrolled?</t>
   </si>
   <si>
     <t>How many degree-seeking undergraduate students of unknown race are enrolled?</t>
@@ -1493,9 +1466,6 @@
   </si>
   <si>
     <t>Rose-Hulman offers bachelors and masters degree</t>
-  </si>
-  <si>
-    <t>The number of degree-seeking first-time freshman  (xor [race] {nonresidence alien}) students enrolled is &lt;value&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">(xor [academic_factor] [non_academic_factor]) is &lt;value&gt; in Rose-Hulman admission decisions </t>
@@ -1705,6 +1675,36 @@
   </si>
   <si>
     <t>What is the minimum college grade point average required for transfer admission?</t>
+  </si>
+  <si>
+    <t>The number of degree-seeking first-time first-year freshman  (xor [race] {nonresidence alien}) students enrolled is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year freshman nonresident aliens are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year freshman hispanics are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year freshman african americans are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year freshman white students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year freshman american indians are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year freshman asians are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year freshman pacific islanders are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year freshman students of two or more races are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year freshman students of unknown race are enrolled?</t>
   </si>
 </sst>
 </file>
@@ -2101,15 +2101,15 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="C2" t="s">
         <v>196</v>
@@ -2117,10 +2117,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="C3" t="s">
         <v>196</v>
@@ -2128,10 +2128,10 @@
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="C4" t="s">
         <v>196</v>
@@ -2139,10 +2139,10 @@
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="C5" t="s">
         <v>196</v>
@@ -2150,10 +2150,10 @@
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="C6" t="s">
         <v>196</v>
@@ -2161,10 +2161,10 @@
     </row>
     <row r="7" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="C7" t="s">
         <v>196</v>
@@ -2172,10 +2172,10 @@
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="C8" t="s">
         <v>196</v>
@@ -2183,10 +2183,10 @@
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="C9" t="s">
         <v>196</v>
@@ -2194,10 +2194,10 @@
     </row>
     <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="C10" t="s">
         <v>196</v>
@@ -2205,10 +2205,10 @@
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
       <c r="C11" t="s">
         <v>196</v>
@@ -2216,10 +2216,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="C12" t="s">
         <v>196</v>
@@ -2227,10 +2227,10 @@
     </row>
     <row r="13" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="C13" t="s">
         <v>196</v>
@@ -2238,10 +2238,10 @@
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="C14" t="s">
         <v>196</v>
@@ -2385,7 +2385,7 @@
         <v>266</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2557,12 +2557,12 @@
       </c>
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>266</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -2694,7 +2694,7 @@
         <v>266</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2801,7 +2801,7 @@
         <v>89</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2871,7 +2871,7 @@
         <v>266</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -2937,7 +2937,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
       <c r="B2" s="4">
         <v>350</v>
@@ -2945,7 +2945,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="B3" s="4">
         <v>296</v>
@@ -2953,7 +2953,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>60</v>
@@ -2961,7 +2961,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>61</v>
@@ -2996,7 +2996,7 @@
         <v>33</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -3092,7 +3092,7 @@
         <v>58</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -3124,7 +3124,7 @@
         <v>29</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -3156,7 +3156,7 @@
         <v>37</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -3188,7 +3188,7 @@
         <v>46</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -3220,7 +3220,7 @@
         <v>59</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -3242,7 +3242,7 @@
         <v>266</v>
       </c>
       <c r="B40" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -3306,12 +3306,12 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>485</v>
+        <v>475</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>98</v>
@@ -3322,7 +3322,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>99</v>
@@ -3333,7 +3333,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>487</v>
+        <v>477</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>100</v>
@@ -3344,7 +3344,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>488</v>
+        <v>478</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>101</v>
@@ -3355,7 +3355,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>489</v>
+        <v>479</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>102</v>
@@ -3366,7 +3366,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>490</v>
+        <v>480</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>103</v>
@@ -3377,7 +3377,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>491</v>
+        <v>481</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>109</v>
@@ -3388,7 +3388,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>492</v>
+        <v>482</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>109</v>
@@ -3399,7 +3399,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>109</v>
@@ -3410,10 +3410,10 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>503</v>
+        <v>493</v>
       </c>
       <c r="C11" t="s">
         <v>196</v>
@@ -3421,10 +3421,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>504</v>
+        <v>494</v>
       </c>
       <c r="C12" t="s">
         <v>196</v>
@@ -3449,7 +3449,7 @@
         <v>266</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>502</v>
+        <v>492</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -3517,7 +3517,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>122</v>
@@ -3525,7 +3525,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>497</v>
+        <v>487</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>123</v>
@@ -3533,7 +3533,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>124</v>
@@ -3541,7 +3541,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>125</v>
@@ -3549,7 +3549,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>109</v>
@@ -3557,7 +3557,7 @@
     </row>
     <row r="7" spans="1:2" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>501</v>
+        <v>491</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>126</v>
@@ -3581,7 +3581,7 @@
         <v>266</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>505</v>
+        <v>495</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -3625,7 +3625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CD6236-1D5E-43C4-8447-268AAEF1A0C5}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3642,7 +3642,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3754,7 +3754,7 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>543</v>
+        <v>533</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>159</v>
@@ -3765,10 +3765,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>544</v>
+        <v>534</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C13" t="s">
         <v>196</v>
@@ -3823,7 +3823,7 @@
         <v>164</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C18" t="s">
         <v>196</v>
@@ -3834,7 +3834,7 @@
         <v>165</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="C19" t="s">
         <v>196</v>
@@ -3856,7 +3856,7 @@
         <v>147</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C21" t="s">
         <v>196</v>
@@ -3970,7 +3970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>132</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>133</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>134</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>266</v>
       </c>
       <c r="B10" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4075,15 +4075,15 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="C2" t="s">
         <v>196</v>
@@ -4091,10 +4091,10 @@
     </row>
     <row r="3" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="C3" t="s">
         <v>196</v>
@@ -4419,7 +4419,7 @@
         <v>266</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>541</v>
+        <v>531</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -4483,7 +4483,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -4736,7 +4736,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
@@ -4869,170 +4869,170 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -5054,7 +5054,7 @@
         <v>266</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -5118,12 +5118,12 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="B2" s="6">
         <v>466</v>
@@ -5134,7 +5134,7 @@
     </row>
     <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B3" s="6">
         <v>360</v>
@@ -5145,7 +5145,7 @@
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="B4" s="6">
         <v>360</v>
@@ -5156,7 +5156,7 @@
     </row>
     <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="B5" s="6">
         <v>357</v>
@@ -5167,7 +5167,7 @@
     </row>
     <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="B6" s="6">
         <v>236</v>
@@ -5178,7 +5178,7 @@
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="B7" s="6">
         <v>168</v>
@@ -5189,7 +5189,7 @@
     </row>
     <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="B8" s="6">
         <v>124</v>
@@ -5200,10 +5200,10 @@
     </row>
     <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="C9" t="s">
         <v>196</v>
@@ -5211,10 +5211,10 @@
     </row>
     <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="C10" t="s">
         <v>196</v>
@@ -5222,10 +5222,10 @@
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="C11" t="s">
         <v>196</v>
@@ -5233,10 +5233,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="C12" t="s">
         <v>196</v>
@@ -5244,10 +5244,10 @@
     </row>
     <row r="13" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="C13" t="s">
         <v>196</v>
@@ -5255,10 +5255,10 @@
     </row>
     <row r="14" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="C14" t="s">
         <v>196</v>
@@ -5266,10 +5266,10 @@
     </row>
     <row r="15" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="C15" t="s">
         <v>196</v>
@@ -5277,10 +5277,10 @@
     </row>
     <row r="16" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C16" t="s">
         <v>196</v>
@@ -5288,10 +5288,10 @@
     </row>
     <row r="17" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C17" t="s">
         <v>196</v>
@@ -5370,15 +5370,15 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="C2" t="s">
         <v>196</v>
@@ -5386,7 +5386,7 @@
     </row>
     <row r="3" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="B3" s="4">
         <v>1151</v>
@@ -5397,7 +5397,7 @@
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="B4" s="4">
         <v>1150</v>
@@ -5408,7 +5408,7 @@
     </row>
     <row r="5" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="B5" s="4">
         <v>1144</v>
@@ -5419,7 +5419,7 @@
     </row>
     <row r="6" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="B6" s="4">
         <v>829</v>
@@ -5430,7 +5430,7 @@
     </row>
     <row r="7" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="B7" s="4">
         <v>1009</v>
@@ -5441,7 +5441,7 @@
     </row>
     <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="B8" s="4">
         <v>284</v>
@@ -5452,7 +5452,7 @@
     </row>
     <row r="9" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>60</v>
@@ -5463,10 +5463,10 @@
     </row>
     <row r="10" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="C10" t="s">
         <v>196</v>
@@ -5474,10 +5474,10 @@
     </row>
     <row r="11" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="C11" t="s">
         <v>196</v>
@@ -5485,10 +5485,10 @@
     </row>
     <row r="12" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="C12" t="s">
         <v>196</v>
@@ -5496,10 +5496,10 @@
     </row>
     <row r="13" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>506</v>
+        <v>496</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="C13" t="s">
         <v>196</v>
@@ -5507,32 +5507,32 @@
     </row>
     <row r="14" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="C14" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="C15" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C16" t="s">
         <v>196</v>
@@ -5540,10 +5540,10 @@
     </row>
     <row r="17" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C17" t="s">
         <v>196</v>
@@ -5623,12 +5623,12 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="B2" s="4">
         <v>6</v>
@@ -5639,7 +5639,7 @@
     </row>
     <row r="3" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="B3" s="4">
         <v>5</v>
@@ -5650,7 +5650,7 @@
     </row>
     <row r="4" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>263</v>
@@ -5661,7 +5661,7 @@
     </row>
     <row r="5" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>263</v>
@@ -5672,7 +5672,7 @@
     </row>
     <row r="6" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="B6" s="4">
         <v>2</v>
@@ -5683,7 +5683,7 @@
     </row>
     <row r="7" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="B7" s="4">
         <v>5</v>
@@ -5694,7 +5694,7 @@
     </row>
     <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
@@ -5705,10 +5705,10 @@
     </row>
     <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="C9" t="s">
         <v>196</v>
@@ -5716,10 +5716,10 @@
     </row>
     <row r="10" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="C10" t="s">
         <v>196</v>
@@ -5727,10 +5727,10 @@
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="C11" t="s">
         <v>196</v>
@@ -5738,10 +5738,10 @@
     </row>
     <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="C12" t="s">
         <v>196</v>
@@ -5749,10 +5749,10 @@
     </row>
     <row r="13" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="C13" t="s">
         <v>196</v>
@@ -5760,10 +5760,10 @@
     </row>
     <row r="14" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="C14" t="s">
         <v>196</v>
@@ -5771,10 +5771,10 @@
     </row>
     <row r="15" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="C15" t="s">
         <v>196</v>
@@ -5782,10 +5782,10 @@
     </row>
     <row r="16" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C16" t="s">
         <v>196</v>
@@ -5793,10 +5793,10 @@
     </row>
     <row r="17" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C17" t="s">
         <v>196</v>
@@ -5877,7 +5877,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>509</v>
+        <v>499</v>
       </c>
       <c r="B2">
         <v>33</v>
@@ -5885,7 +5885,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>510</v>
+        <v>500</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5893,7 +5893,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>511</v>
+        <v>501</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -5901,7 +5901,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>512</v>
+        <v>502</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5926,7 +5926,7 @@
         <v>266</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>513</v>
+        <v>503</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -5990,7 +5990,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -5998,7 +5998,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -6006,7 +6006,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="B4">
         <v>137</v>
@@ -6014,7 +6014,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -6039,7 +6039,7 @@
         <v>266</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>507</v>
+        <v>497</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -6103,7 +6103,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="B2">
         <v>182</v>
@@ -6111,7 +6111,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -6119,7 +6119,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -6127,7 +6127,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -6135,7 +6135,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -6143,7 +6143,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -6151,7 +6151,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -6159,7 +6159,7 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -6184,7 +6184,7 @@
         <v>266</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>508</v>
+        <v>498</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -6247,15 +6247,15 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
       <c r="C2" t="s">
         <v>196</v>
@@ -6263,10 +6263,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="C3" t="s">
         <v>196</v>
@@ -6350,7 +6350,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B2">
         <v>226</v>
@@ -6358,7 +6358,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B3">
         <v>104</v>
@@ -6366,7 +6366,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B4">
         <v>93</v>
@@ -6374,7 +6374,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B5">
         <v>1295</v>
@@ -6382,7 +6382,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -6390,7 +6390,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B7">
         <v>127</v>
@@ -6398,7 +6398,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -6406,7 +6406,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B9">
         <v>99</v>
@@ -6414,7 +6414,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B10">
         <v>22</v>
@@ -6438,7 +6438,7 @@
         <v>266</v>
       </c>
       <c r="B13" t="s">
-        <v>540</v>
+        <v>530</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -6475,10 +6475,10 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="B18" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -6510,15 +6510,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
       <c r="B2" t="s">
-        <v>525</v>
+        <v>515</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="B3">
         <v>76</v>
@@ -6526,7 +6526,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="B4">
         <v>216</v>
@@ -6534,7 +6534,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="B5">
         <v>129</v>
@@ -6542,7 +6542,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -6550,7 +6550,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -6558,7 +6558,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -6566,7 +6566,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>524</v>
+        <v>514</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -6647,7 +6647,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -6655,7 +6655,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
       <c r="B3">
         <v>33</v>
@@ -6663,7 +6663,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -6671,7 +6671,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -6679,7 +6679,7 @@
     </row>
     <row r="6" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -6687,7 +6687,7 @@
     </row>
     <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -6695,7 +6695,7 @@
     </row>
     <row r="8" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -6742,13 +6742,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8ED044F-2B62-42B7-A288-F87892E20B00}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="83.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="97.77734375" customWidth="1"/>
     <col min="2" max="2" width="93.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.88671875" customWidth="1"/>
   </cols>
@@ -6763,7 +6763,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>303</v>
+        <v>536</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -6771,7 +6771,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>305</v>
+        <v>537</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -6779,7 +6779,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>307</v>
+        <v>538</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -6787,7 +6787,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>309</v>
+        <v>539</v>
       </c>
       <c r="B5">
         <v>356</v>
@@ -6795,7 +6795,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>311</v>
+        <v>540</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -6803,7 +6803,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>313</v>
+        <v>541</v>
       </c>
       <c r="B7">
         <v>36</v>
@@ -6811,7 +6811,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>315</v>
+        <v>542</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -6819,7 +6819,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>317</v>
+        <v>543</v>
       </c>
       <c r="B9">
         <v>31</v>
@@ -6827,7 +6827,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>319</v>
+        <v>544</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -6851,7 +6851,7 @@
         <v>266</v>
       </c>
       <c r="B13" t="s">
-        <v>475</v>
+        <v>535</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -6888,10 +6888,10 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="B18" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -6955,7 +6955,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>242</v>
@@ -7078,7 +7078,7 @@
         <v>267</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -7086,7 +7086,7 @@
         <v>266</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>542</v>
+        <v>532</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -7350,7 +7350,7 @@
         <v>266</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -7380,7 +7380,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
work on input data from client
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\irpa_db\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D6AA49-AF07-43BB-B6AA-5FE2CFDADF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABC3F10-5A6D-4541-B4EC-C361E1CE9CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -44,6 +44,7 @@
     <sheet name="Faculty And Class Size_Other" sheetId="26" r:id="rId29"/>
     <sheet name="Faculty And Class Size_Section" sheetId="31" r:id="rId30"/>
     <sheet name="Faculy And Class Size_Subsectio" sheetId="32" r:id="rId31"/>
+    <sheet name="Degree Conferred" sheetId="33" r:id="rId32"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="586">
   <si>
     <t>Answer</t>
   </si>
@@ -1705,6 +1706,129 @@
   </si>
   <si>
     <t>How many degree-seeking first-time first-year freshman students of unknown race are enrolled?</t>
+  </si>
+  <si>
+    <t>How many foreign language units are required for admission?</t>
+  </si>
+  <si>
+    <t>How many social studies units are required for admission?</t>
+  </si>
+  <si>
+    <t>How many history units are required for admission?</t>
+  </si>
+  <si>
+    <t>How many academic elective units are required for admission?</t>
+  </si>
+  <si>
+    <t>How many computer science units are required for admission?</t>
+  </si>
+  <si>
+    <t>How many visual/performing art units are required for admission?</t>
+  </si>
+  <si>
+    <t>What other units are required for admission?</t>
+  </si>
+  <si>
+    <t>How many English units are required for admission?</t>
+  </si>
+  <si>
+    <t>How many Mathematics units are required for admission?</t>
+  </si>
+  <si>
+    <t>How many science units are required for admission?</t>
+  </si>
+  <si>
+    <t>Of the previous units, how many lab units required for admission?</t>
+  </si>
+  <si>
+    <t>How many English units are recommended for admission?</t>
+  </si>
+  <si>
+    <t>How many Mathematics units are recommended for admission?</t>
+  </si>
+  <si>
+    <t>How many science units are recommended for admission?</t>
+  </si>
+  <si>
+    <t>How many foreign language units are recommended for admission?</t>
+  </si>
+  <si>
+    <t>How many social studies units are recommended for admission?</t>
+  </si>
+  <si>
+    <t>How many history units are recommended for admission?</t>
+  </si>
+  <si>
+    <t>How many academic elective units are recommended for admission?</t>
+  </si>
+  <si>
+    <t>How many computer science units are recommended for admission?</t>
+  </si>
+  <si>
+    <t>How many visual/performing art units are recommended for admission?</t>
+  </si>
+  <si>
+    <t>What other units are recommended for admission?</t>
+  </si>
+  <si>
+    <t>How many Computer and information scienses degrees are conferred?</t>
+  </si>
+  <si>
+    <t>There are 15.7% bachelor's degrees conferred are Computer and information scienses, CIP is 11</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>How many Engineering degrees are conferred?</t>
+  </si>
+  <si>
+    <t>There are 73.1% bachelor's degrees conferred are Engineering , CIP is 14</t>
+  </si>
+  <si>
+    <t>How many Biological/life sciences degrees are conferred?</t>
+  </si>
+  <si>
+    <t>There are 2.2% bachelor's degrees conferred are  Biological/life sciences , CIP is 26</t>
+  </si>
+  <si>
+    <t>How many Mathematics and statistics degrees are conferred?</t>
+  </si>
+  <si>
+    <t>There are 5.2% bachelor's degrees conferred are Mathematics and statistics, CIP is 27</t>
+  </si>
+  <si>
+    <t>How many Interdisciplinary studies degrees are conferred?</t>
+  </si>
+  <si>
+    <t>There are 0.7% bachelor's degrees conferred are Interdisciplinary studies, CIP is 30</t>
+  </si>
+  <si>
+    <t>How many Physical sciences degrees are conferred?</t>
+  </si>
+  <si>
+    <t>There are 3.0% bachelor's degrees conferred are Physical sciences, CIP is 40</t>
+  </si>
+  <si>
+    <t>How many Social sciences degrees are conferred?</t>
+  </si>
+  <si>
+    <t>There are 0.2% bachelor's degrees conferred are Social sciences, CIP is 45</t>
+  </si>
+  <si>
+    <t>Of previous units, how many lab units are recommended for admission?</t>
+  </si>
+  <si>
+    <t>What other units are required for admission? (please specify)</t>
+  </si>
+  <si>
+    <t>No other additional units are required for admission</t>
+  </si>
+  <si>
+    <t>The number of [subject] units required to be taken by students during high school for admission to Rose-Hulman  is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>The number of [subject] units recommended to be taken by students during high school for admission to Rose-Hulman  is &lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -2082,8 +2206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E422E2F-D9FA-411F-968E-DE340F994DF5}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6491,7 +6615,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6738,12 +6862,120 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A321CDB-4432-42F8-8542-C3389F944EAE}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="34.21875" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>566</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>567</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>580</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>568</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8ED044F-2B62-42B7-A288-F87892E20B00}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6903,8 +7135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7606B2B-8397-4A8E-AF38-C293D77D8867}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7129,28 +7361,386 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DC138E-AAA1-4452-BC05-6992F74BED09}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="32.77734375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="B2" s="5">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="B3" s="5">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="C13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50A1A77-FCFF-4BA2-80DC-49E66C3D11B3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="37.88671875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>581</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fixed bugs with template and discrete range, work on percentaeg
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -8,43 +8,44 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\irpa_db\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABC3F10-5A6D-4541-B4EC-C361E1CE9CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8A6E35-A124-4B34-854C-515D9610A26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
     <sheet name="Enrollment_General" sheetId="12" r:id="rId2"/>
     <sheet name="Enrollment_Race Undergraduate" sheetId="16" r:id="rId3"/>
-    <sheet name="Enrollment_Race Freshman" sheetId="13" r:id="rId4"/>
+    <sheet name="Enrollment_Race First time year" sheetId="13" r:id="rId4"/>
     <sheet name="Cohort" sheetId="10" r:id="rId5"/>
     <sheet name="High School Units_Required" sheetId="29" r:id="rId6"/>
     <sheet name="High School Units_Recommended" sheetId="28" r:id="rId7"/>
     <sheet name="Basis For Selection" sheetId="1" r:id="rId8"/>
     <sheet name="Admission Policies" sheetId="9" r:id="rId9"/>
-    <sheet name="Freshman Profile_SAT Score Comp" sheetId="14" r:id="rId10"/>
-    <sheet name="Freshman Profile_SAT Score Sub " sheetId="3" r:id="rId11"/>
-    <sheet name="Freshman Profile_ACT score comp" sheetId="15" r:id="rId12"/>
-    <sheet name="Freshman Profile_ACT Score sub" sheetId="11" r:id="rId13"/>
-    <sheet name="Freshman Profile_Percentile" sheetId="2" r:id="rId14"/>
-    <sheet name="Freshman Profile_GPA" sheetId="4" r:id="rId15"/>
-    <sheet name="Freshman Profile_Class Rank" sheetId="18" r:id="rId16"/>
-    <sheet name="Transfer Admission_General" sheetId="5" r:id="rId17"/>
-    <sheet name="Transfer Admission_Statistic" sheetId="17" r:id="rId18"/>
-    <sheet name="Academic Offering Policy" sheetId="27" r:id="rId19"/>
-    <sheet name="Student Life_Categories" sheetId="7" r:id="rId20"/>
-    <sheet name="Student Life_Offered" sheetId="8" r:id="rId21"/>
-    <sheet name="Financial Aid_Awarded" sheetId="19" r:id="rId22"/>
-    <sheet name="Financial Aid_Awarded Freshman" sheetId="20" r:id="rId23"/>
-    <sheet name="Financial Aid_Awarded Undergrad" sheetId="21" r:id="rId24"/>
-    <sheet name="Financial Aid_Awarded Part-Time" sheetId="22" r:id="rId25"/>
-    <sheet name="Faculty And Class Size_Race" sheetId="30" r:id="rId26"/>
-    <sheet name="Faculty And Class Size_Gender" sheetId="24" r:id="rId27"/>
-    <sheet name="Faculty And Class Size_Degree" sheetId="25" r:id="rId28"/>
-    <sheet name="Faculty And Class Size_Other" sheetId="26" r:id="rId29"/>
-    <sheet name="Faculty And Class Size_Section" sheetId="31" r:id="rId30"/>
-    <sheet name="Faculy And Class Size_Subsectio" sheetId="32" r:id="rId31"/>
-    <sheet name="Degree Conferred" sheetId="33" r:id="rId32"/>
+    <sheet name="Freshman Profile_SAT comp range" sheetId="14" r:id="rId10"/>
+    <sheet name="Freshman Profile_SAT sub range " sheetId="3" r:id="rId11"/>
+    <sheet name="Freshman Profile_ACT comp range" sheetId="15" r:id="rId12"/>
+    <sheet name="Freshman Profile_ACT sub range" sheetId="11" r:id="rId13"/>
+    <sheet name="Freshman Profile_Submit" sheetId="34" r:id="rId14"/>
+    <sheet name="Freshman Profile_Percentile" sheetId="2" r:id="rId15"/>
+    <sheet name="Freshman Profile_GPA" sheetId="4" r:id="rId16"/>
+    <sheet name="Freshman Profile_Class Rank" sheetId="18" r:id="rId17"/>
+    <sheet name="Transfer Admission_General" sheetId="5" r:id="rId18"/>
+    <sheet name="Transfer Admission_Statistic" sheetId="17" r:id="rId19"/>
+    <sheet name="Academic Offering Policy" sheetId="27" r:id="rId20"/>
+    <sheet name="Student Life_Categories" sheetId="7" r:id="rId21"/>
+    <sheet name="Student Life_Offered" sheetId="8" r:id="rId22"/>
+    <sheet name="Financial Aid_Awarded" sheetId="19" r:id="rId23"/>
+    <sheet name="Financial Aid_Awarded Freshman" sheetId="20" r:id="rId24"/>
+    <sheet name="Financial Aid_Awarded Undergrad" sheetId="21" r:id="rId25"/>
+    <sheet name="Financial Aid_Awarded Part-Time" sheetId="22" r:id="rId26"/>
+    <sheet name="Faculty And Class Size_Race" sheetId="30" r:id="rId27"/>
+    <sheet name="Faculty And Class Size_Gender" sheetId="24" r:id="rId28"/>
+    <sheet name="Faculty And Class Size_Degree" sheetId="25" r:id="rId29"/>
+    <sheet name="Faculty And Class Size_Other" sheetId="26" r:id="rId30"/>
+    <sheet name="Faculty And Class Size_Section" sheetId="31" r:id="rId31"/>
+    <sheet name="Faculty And Class Size_Subsec" sheetId="32" r:id="rId32"/>
+    <sheet name="Degree Conferred" sheetId="33" r:id="rId33"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="591">
   <si>
     <t>Answer</t>
   </si>
@@ -1402,9 +1403,6 @@
     <t>What is the number of degree-seeking full-time full-time freshman students who applied for need-based financial aid</t>
   </si>
   <si>
-    <t>The (xor [percentile] [aggregation]) score for [standarized_test] [subject] is &lt;value&gt;</t>
-  </si>
-  <si>
     <t>What special study programs are offered at Rose-Hulman?</t>
   </si>
   <si>
@@ -1478,9 +1476,6 @@
     <t xml:space="preserve">The percentage of freshman students with sat (xor [test_component] [subject]) score (xor {[range] [number] and [number]} {[range] [number]}) is &lt;value&gt; </t>
   </si>
   <si>
-    <t xml:space="preserve">The percentage of freshman students with act composite (xor {[range] [number] and [number]} {[range] [number]}) is &lt;value&gt; </t>
-  </si>
-  <si>
     <t xml:space="preserve">The percentage of freshman students with act (xor [test_component] [subject]) score (xor {[range] [number] and [number]} {[range] [number]}) is &lt;value&gt; </t>
   </si>
   <si>
@@ -1545,9 +1540,6 @@
   </si>
   <si>
     <t>What is the percentage of freshman students who submitted high school class rank?</t>
-  </si>
-  <si>
-    <t>(xor {The percentage of freshman students with gpa (xor {[range] [number] and [number]} {[range] [number]}) is &lt;value&gt;}</t>
   </si>
   <si>
     <t xml:space="preserve"> The average high school gpa for freshman student who submitted gpa is 4.02</t>
@@ -1678,36 +1670,6 @@
     <t>What is the minimum college grade point average required for transfer admission?</t>
   </si>
   <si>
-    <t>The number of degree-seeking first-time first-year freshman  (xor [race] {nonresidence alien}) students enrolled is &lt;value&gt;</t>
-  </si>
-  <si>
-    <t>How many degree-seeking first-time first-year freshman nonresident aliens are enrolled?</t>
-  </si>
-  <si>
-    <t>How many degree-seeking first-time first-year freshman hispanics are enrolled?</t>
-  </si>
-  <si>
-    <t>How many degree-seeking first-time first-year freshman african americans are enrolled?</t>
-  </si>
-  <si>
-    <t>How many degree-seeking first-time first-year freshman white students are enrolled?</t>
-  </si>
-  <si>
-    <t>How many degree-seeking first-time first-year freshman american indians are enrolled?</t>
-  </si>
-  <si>
-    <t>How many degree-seeking first-time first-year freshman asians are enrolled?</t>
-  </si>
-  <si>
-    <t>How many degree-seeking first-time first-year freshman pacific islanders are enrolled?</t>
-  </si>
-  <si>
-    <t>How many degree-seeking first-time first-year freshman students of two or more races are enrolled?</t>
-  </si>
-  <si>
-    <t>How many degree-seeking first-time first-year freshman students of unknown race are enrolled?</t>
-  </si>
-  <si>
     <t>How many foreign language units are required for admission?</t>
   </si>
   <si>
@@ -1829,6 +1791,60 @@
   </si>
   <si>
     <t>The number of [subject] units recommended to be taken by students during high school for admission to Rose-Hulman  is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>How many degree-seeking undergraduate students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year nonresident aliens are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year hispanics are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year african americans are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year white students are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year asians are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year pacific islanders are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year students of two or more races are enrolled?</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year students of unknown race are enrolled?</t>
+  </si>
+  <si>
+    <t>The number of degree-seeking first-time first-year  (xor [race] {nonresidence alien}) students enrolled is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>How many degree-seeking first-time first-year american indians are enrolled?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The percentage of freshman students with act composite score (xor {[range] [number] and [number]} {[range] [number]}) is &lt;value&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>The (xor [aggregation] [percentile]) score [standarized_test] [subject] for freshmen is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>296</t>
+  </si>
+  <si>
+    <t>The (xor number [*percentage]) of freshman students who submitted [standarized_test] score is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>The percentage of freshman students with gpa (xor {[range] [number] and [number]} {[range] [number]}) is &lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -2233,7 +2249,7 @@
         <v>419</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C2" t="s">
         <v>196</v>
@@ -2241,10 +2257,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>452</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>453</v>
       </c>
       <c r="C3" t="s">
         <v>196</v>
@@ -2255,7 +2271,7 @@
         <v>421</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C4" t="s">
         <v>196</v>
@@ -2266,7 +2282,7 @@
         <v>420</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C5" t="s">
         <v>196</v>
@@ -2277,7 +2293,7 @@
         <v>422</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C6" t="s">
         <v>196</v>
@@ -2288,7 +2304,7 @@
         <v>423</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C7" t="s">
         <v>196</v>
@@ -2299,7 +2315,7 @@
         <v>424</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C8" t="s">
         <v>196</v>
@@ -2307,10 +2323,10 @@
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>459</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>460</v>
       </c>
       <c r="C9" t="s">
         <v>196</v>
@@ -2321,7 +2337,7 @@
         <v>425</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C10" t="s">
         <v>196</v>
@@ -2332,7 +2348,7 @@
         <v>426</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C11" t="s">
         <v>196</v>
@@ -2343,7 +2359,7 @@
         <v>427</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C12" t="s">
         <v>196</v>
@@ -2354,7 +2370,7 @@
         <v>428</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C13" t="s">
         <v>196</v>
@@ -2365,7 +2381,7 @@
         <v>429</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C14" t="s">
         <v>196</v>
@@ -2426,7 +2442,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2509,7 +2525,7 @@
         <v>266</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2554,7 +2570,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2686,7 +2702,7 @@
         <v>266</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -2735,7 +2751,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2813,12 +2829,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>266</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>469</v>
+        <v>584</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2860,7 +2876,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20057133-7837-4203-86B9-F46D32350538}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
@@ -2995,18 +3011,21 @@
         <v>266</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>268</v>
       </c>
       <c r="B17" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>269</v>
       </c>
@@ -3014,7 +3033,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>273</v>
       </c>
@@ -3022,7 +3041,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>271</v>
       </c>
@@ -3037,367 +3056,109 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3892E9F-E7EA-42B9-AE4C-1275BBD6A387}">
-  <dimension ref="A1:B44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998E6B56-71DD-4A78-89DB-D3F23672C01B}">
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="105" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="81.21875" customWidth="1"/>
-    <col min="2" max="2" width="68.21875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" customWidth="1"/>
+    <col min="1" max="1" width="44.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="B4" s="6">
         <v>350</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="B3" s="4">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>61</v>
+      <c r="A5" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1270</v>
+      <c r="A6" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="4">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="4">
-        <v>650</v>
+      <c r="A7" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>316</v>
+      <c r="A9" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1355</v>
+      <c r="A10" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="4">
-        <v>650</v>
+      <c r="A11" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="4">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="4">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="4">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="4">
-        <v>1352</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="4">
-        <v>1352</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="4">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="4">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="4">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="4">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="4">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="4">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="4">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="4">
-        <v>31.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="4">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="4">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="B38" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="B39"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="B40" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="B41" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="B42" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B43" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="A12" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B12" s="5" t="s">
         <v>234</v>
       </c>
     </row>
@@ -3408,11 +3169,350 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3892E9F-E7EA-42B9-AE4C-1275BBD6A387}">
+  <dimension ref="A1:B40"/>
+  <sheetViews>
+    <sheetView zoomScale="105" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="81.21875" customWidth="1"/>
+    <col min="2" max="2" width="74.109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="4">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="4">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="4">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="4">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="4">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="4">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="4">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="4">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B34" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="B35"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B36" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B37" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B38" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B39" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B40" t="s">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB852AE-A4C7-4284-9FBD-1CEEB9311916}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3435,7 +3535,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>98</v>
@@ -3446,7 +3546,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>99</v>
@@ -3457,7 +3557,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>100</v>
@@ -3468,7 +3568,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>101</v>
@@ -3479,7 +3579,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>102</v>
@@ -3490,7 +3590,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>103</v>
@@ -3501,7 +3601,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>109</v>
@@ -3512,7 +3612,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>109</v>
@@ -3523,7 +3623,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>109</v>
@@ -3534,10 +3634,10 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C11" t="s">
         <v>196</v>
@@ -3545,10 +3645,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="C12" t="s">
         <v>196</v>
@@ -3573,7 +3673,7 @@
         <v>266</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>492</v>
+        <v>590</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -3617,7 +3717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBBFCBD-BE53-4EBE-BC28-AF1024B4BD2D}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -3641,7 +3741,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>122</v>
@@ -3649,7 +3749,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>123</v>
@@ -3657,7 +3757,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>124</v>
@@ -3665,7 +3765,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>125</v>
@@ -3673,7 +3773,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>109</v>
@@ -3681,7 +3781,7 @@
     </row>
     <row r="7" spans="1:2" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>126</v>
@@ -3705,7 +3805,7 @@
         <v>266</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -3745,7 +3845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CD6236-1D5E-43C4-8447-268AAEF1A0C5}">
   <dimension ref="A1:C28"/>
   <sheetViews>
@@ -3878,7 +3978,7 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>159</v>
@@ -3889,7 +3989,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>318</v>
@@ -4048,7 +4148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869E4568-D908-477D-923D-F4116B90EDC7}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -4136,7 +4236,7 @@
         <v>266</v>
       </c>
       <c r="B10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4173,109 +4273,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40ABA4F2-212D-4CBD-893A-EB2683BB9A32}">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="74.88671875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>445</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="C2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="C3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="B4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="B5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="B7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B8" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4543,7 +4540,7 @@
         <v>266</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -4585,6 +4582,109 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40ABA4F2-212D-4CBD-893A-EB2683BB9A32}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="74.88671875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="C2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="C3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="B5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B8" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AECD6F-4371-4391-B58E-E510CF964736}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -4837,7 +4937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD4CE82-100F-475B-B66F-A9CBAA32385B}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -4969,7 +5069,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E00C0EE-B5EA-4C5D-A3F6-0409760A68CF}">
   <dimension ref="A1:B29"/>
   <sheetViews>
@@ -5065,7 +5165,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>387</v>
@@ -5073,7 +5173,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>388</v>
@@ -5081,7 +5181,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>389</v>
@@ -5089,7 +5189,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>381</v>
@@ -5097,7 +5197,7 @@
     </row>
     <row r="15" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>381</v>
@@ -5105,7 +5205,7 @@
     </row>
     <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>381</v>
@@ -5178,7 +5278,7 @@
         <v>266</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -5219,7 +5319,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD85EB1-BDB8-4AEB-99D1-57DF875DFEB5}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -5471,7 +5571,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE4F375-28FB-4634-A90F-E29F4CD5ADA1}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -5620,7 +5720,7 @@
     </row>
     <row r="13" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>410</v>
@@ -5724,7 +5824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EA6128-27F4-4911-A1F0-865B26420EEF}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -5977,12 +6077,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680EF845-E97A-4774-A116-33BCEE8AAAAA}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6001,7 +6101,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B2">
         <v>33</v>
@@ -6009,7 +6109,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -6017,7 +6117,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -6025,7 +6125,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -6050,7 +6150,7 @@
         <v>266</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -6087,15 +6187,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2A9967-94EA-41CF-ACB5-C81483AD239D}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6163,7 +6264,7 @@
         <v>266</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -6203,7 +6304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2758D6-F888-4498-88A0-7DFBF7091CA2}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -6308,7 +6409,7 @@
         <v>266</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -6348,7 +6449,167 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354727B8-DF4A-4CB3-BBB4-023F92A30B71}">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="82.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="88.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B4">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B5">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B7">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B9">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B11" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B13" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B14" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B16" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B18" t="s">
+        <v>573</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ED34DA-E2CB-4859-9A96-48DF7AE0B7A7}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -6376,10 +6637,10 @@
     </row>
     <row r="2" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C2" t="s">
         <v>196</v>
@@ -6390,7 +6651,7 @@
         <v>442</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C3" t="s">
         <v>196</v>
@@ -6450,167 +6711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354727B8-DF4A-4CB3-BBB4-023F92A30B71}">
-  <dimension ref="A1:B18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="82.44140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="88.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="B2">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="B3">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="B4">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B5">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="B7">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="B9">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B10">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="B11" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="B13" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="B14" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="B15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B16" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B17" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="B18" t="s">
-        <v>312</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F6BE80-AC56-42ED-87D6-9266FD24F810}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -6634,15 +6735,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B2" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B3">
         <v>76</v>
@@ -6650,7 +6751,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B4">
         <v>216</v>
@@ -6658,7 +6759,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B5">
         <v>129</v>
@@ -6666,7 +6767,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -6674,7 +6775,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -6682,7 +6783,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -6690,7 +6791,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -6747,12 +6848,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA74624B-4AE3-43E9-9C9C-696C43DB0CE5}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6771,7 +6872,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -6779,7 +6880,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B3">
         <v>33</v>
@@ -6787,7 +6888,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -6795,7 +6896,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -6803,7 +6904,7 @@
     </row>
     <row r="6" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -6811,7 +6912,7 @@
     </row>
     <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -6819,7 +6920,7 @@
     </row>
     <row r="8" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -6862,7 +6963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A321CDB-4432-42F8-8542-C3389F944EAE}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -6890,79 +6991,79 @@
     </row>
     <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>566</v>
+        <v>553</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>569</v>
+        <v>556</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>570</v>
+        <v>557</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>571</v>
+        <v>558</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>572</v>
+        <v>559</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>573</v>
+        <v>560</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>574</v>
+        <v>561</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>575</v>
+        <v>562</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>576</v>
+        <v>563</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>577</v>
+        <v>564</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>578</v>
+        <v>565</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>579</v>
+        <v>566</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>580</v>
+        <v>567</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>
@@ -6975,7 +7076,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B18"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6995,7 +7096,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>536</v>
+        <v>574</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -7003,7 +7104,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>537</v>
+        <v>575</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -7011,7 +7112,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>538</v>
+        <v>576</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -7019,7 +7120,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>539</v>
+        <v>577</v>
       </c>
       <c r="B5">
         <v>356</v>
@@ -7027,7 +7128,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>540</v>
+        <v>583</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -7035,7 +7136,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>541</v>
+        <v>578</v>
       </c>
       <c r="B7">
         <v>36</v>
@@ -7043,7 +7144,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>542</v>
+        <v>579</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -7051,7 +7152,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>543</v>
+        <v>580</v>
       </c>
       <c r="B9">
         <v>31</v>
@@ -7059,7 +7160,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>544</v>
+        <v>581</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -7083,7 +7184,7 @@
         <v>266</v>
       </c>
       <c r="B13" t="s">
-        <v>535</v>
+        <v>582</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -7115,7 +7216,7 @@
         <v>271</v>
       </c>
       <c r="B17" t="s">
-        <v>234</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -7135,8 +7236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7606B2B-8397-4A8E-AF38-C293D77D8867}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7318,7 +7419,7 @@
         <v>266</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -7363,7 +7464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DC138E-AAA1-4452-BC05-6992F74BED09}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -7382,12 +7483,12 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>552</v>
+        <v>539</v>
       </c>
       <c r="B2" s="5">
         <v>4</v>
@@ -7398,7 +7499,7 @@
     </row>
     <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
       <c r="B3" s="5">
         <v>4</v>
@@ -7409,7 +7510,7 @@
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>554</v>
+        <v>541</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
@@ -7420,7 +7521,7 @@
     </row>
     <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>555</v>
+        <v>542</v>
       </c>
       <c r="B5" s="5">
         <v>3</v>
@@ -7431,7 +7532,7 @@
     </row>
     <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>545</v>
+        <v>532</v>
       </c>
       <c r="B6" s="5">
         <v>0</v>
@@ -7442,7 +7543,7 @@
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>546</v>
+        <v>533</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -7453,7 +7554,7 @@
     </row>
     <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>547</v>
+        <v>534</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -7464,7 +7565,7 @@
     </row>
     <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>548</v>
+        <v>535</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -7475,7 +7576,7 @@
     </row>
     <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>549</v>
+        <v>536</v>
       </c>
       <c r="B10" s="5">
         <v>0</v>
@@ -7486,7 +7587,7 @@
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>550</v>
+        <v>537</v>
       </c>
       <c r="B11" s="5">
         <v>0</v>
@@ -7497,7 +7598,7 @@
     </row>
     <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>551</v>
+        <v>538</v>
       </c>
       <c r="B12" s="5">
         <v>0</v>
@@ -7508,10 +7609,10 @@
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>582</v>
+        <v>569</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>583</v>
+        <v>570</v>
       </c>
       <c r="C13" t="s">
         <v>196</v>
@@ -7535,7 +7636,7 @@
         <v>266</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>584</v>
+        <v>571</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -7600,7 +7701,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>556</v>
+        <v>543</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -7608,7 +7709,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -7616,7 +7717,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>558</v>
+        <v>545</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -7624,7 +7725,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>581</v>
+        <v>568</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -7632,7 +7733,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -7640,7 +7741,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>560</v>
+        <v>547</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -7648,7 +7749,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>561</v>
+        <v>548</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -7656,7 +7757,7 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>562</v>
+        <v>549</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -7664,7 +7765,7 @@
     </row>
     <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>563</v>
+        <v>550</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -7672,7 +7773,7 @@
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>564</v>
+        <v>551</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -7680,7 +7781,7 @@
     </row>
     <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>565</v>
+        <v>552</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -7705,7 +7806,7 @@
         <v>266</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>585</v>
+        <v>572</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -7940,7 +8041,7 @@
         <v>266</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
will began working on fixing issue with template
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\irpa_db\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8A6E35-A124-4B34-854C-515D9610A26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286ABCC5-9B72-43DB-B980-26A9BA6449A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="20" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -35,17 +35,18 @@
     <sheet name="Academic Offering Policy" sheetId="27" r:id="rId20"/>
     <sheet name="Student Life_Categories" sheetId="7" r:id="rId21"/>
     <sheet name="Student Life_Offered" sheetId="8" r:id="rId22"/>
-    <sheet name="Financial Aid_Awarded" sheetId="19" r:id="rId23"/>
-    <sheet name="Financial Aid_Awarded Freshman" sheetId="20" r:id="rId24"/>
-    <sheet name="Financial Aid_Awarded Undergrad" sheetId="21" r:id="rId25"/>
-    <sheet name="Financial Aid_Awarded Part-Time" sheetId="22" r:id="rId26"/>
-    <sheet name="Faculty And Class Size_Race" sheetId="30" r:id="rId27"/>
-    <sheet name="Faculty And Class Size_Gender" sheetId="24" r:id="rId28"/>
-    <sheet name="Faculty And Class Size_Degree" sheetId="25" r:id="rId29"/>
-    <sheet name="Faculty And Class Size_Other" sheetId="26" r:id="rId30"/>
-    <sheet name="Faculty And Class Size_Section" sheetId="31" r:id="rId31"/>
-    <sheet name="Faculty And Class Size_Subsec" sheetId="32" r:id="rId32"/>
-    <sheet name="Degree Conferred" sheetId="33" r:id="rId33"/>
+    <sheet name="Annual Expense" sheetId="35" r:id="rId23"/>
+    <sheet name="Financial Aid_Awarded" sheetId="19" r:id="rId24"/>
+    <sheet name="Financial Aid_Awarded Freshman" sheetId="20" r:id="rId25"/>
+    <sheet name="Financial Aid_Awarded Undergrad" sheetId="21" r:id="rId26"/>
+    <sheet name="Financial Aid_Awarded Part-Time" sheetId="22" r:id="rId27"/>
+    <sheet name="Faculty And Class Size_Race" sheetId="30" r:id="rId28"/>
+    <sheet name="Faculty And Class Size_Gender" sheetId="24" r:id="rId29"/>
+    <sheet name="Faculty And Class Size_Degree" sheetId="25" r:id="rId30"/>
+    <sheet name="Faculty And Class Size_Other" sheetId="26" r:id="rId31"/>
+    <sheet name="Faculty And Class Size_Section" sheetId="31" r:id="rId32"/>
+    <sheet name="Faculty And Class Size_Subsec" sheetId="32" r:id="rId33"/>
+    <sheet name="Degree Conferred" sheetId="33" r:id="rId34"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="624">
   <si>
     <t>Answer</t>
   </si>
@@ -1845,6 +1846,105 @@
   </si>
   <si>
     <t>The percentage of freshman students with gpa (xor {[range] [number] and [number]} {[range] [number]}) is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>What is the URL of your institution's Net price calculator?</t>
+  </si>
+  <si>
+    <t>The Url of Rose-Hulman institution's net price calculator is : https://prod11gbss8.rose-hulman.edu/BanSS/RHIT_NPCALC.P_Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes </t>
+  </si>
+  <si>
+    <t>What is the approximate date of the academic year tuition fee cost releaseing?</t>
+  </si>
+  <si>
+    <t>April 1</t>
+  </si>
+  <si>
+    <t>What is the first year private institution tuition fee cost for first-year or undergraduate students?</t>
+  </si>
+  <si>
+    <t>$49,479</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>What is the required fee for first-year or undergraduate students?</t>
+  </si>
+  <si>
+    <t>$1,035</t>
+  </si>
+  <si>
+    <t>What is the Room and board fee for first-year or undergraduate students?</t>
+  </si>
+  <si>
+    <t>$15,690</t>
+  </si>
+  <si>
+    <t>What is the Room fee only for first-year or undergraduate students?</t>
+  </si>
+  <si>
+    <t>$9,441</t>
+  </si>
+  <si>
+    <t>What is the board fee only for first-year or undergraduate students?</t>
+  </si>
+  <si>
+    <t>$6,249</t>
+  </si>
+  <si>
+    <t>Is there any other fee cost for first-year or undergraduate students?</t>
+  </si>
+  <si>
+    <t>Yes, Freshman Laptop $2,400 (First Fall Term for freshman only)</t>
+  </si>
+  <si>
+    <t>What is the number of credits a student can take for the stated full-time tuition</t>
+  </si>
+  <si>
+    <t>From 12 to 18</t>
+  </si>
+  <si>
+    <t>Does tuition and fee change by year of study?</t>
+  </si>
+  <si>
+    <t>Do tuition and fees changes by undergraduate instructional program?</t>
+  </si>
+  <si>
+    <t>What is the cost of book and supplies for residents?</t>
+  </si>
+  <si>
+    <t>What is the cost of book and supplies for Commuters?</t>
+  </si>
+  <si>
+    <t>What is the cost of room only for Commuters?</t>
+  </si>
+  <si>
+    <t>For commuters not living at home is $9,441</t>
+  </si>
+  <si>
+    <t>What is the cost of board only for Commuters?</t>
+  </si>
+  <si>
+    <t>For commuters  living at home is $900,and for commuters not living at home is $6,249</t>
+  </si>
+  <si>
+    <t>how much is other cost for residents?</t>
+  </si>
+  <si>
+    <t>$1,557</t>
+  </si>
+  <si>
+    <t>how much is other cost for commuters?</t>
+  </si>
+  <si>
+    <t>How much does a credit cost?</t>
+  </si>
+  <si>
+    <t>per-credit-hour charges $1,444</t>
   </si>
 </sst>
 </file>
@@ -1907,7 +2007,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1937,6 +2037,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3511,7 +3614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB852AE-A4C7-4284-9FBD-1CEEB9311916}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -5070,6 +5173,231 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD284E4D-E296-45CE-8E65-A3C009D67DE2}">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.21875" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>591</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>592</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>594</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>595</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>596</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>597</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>599</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>600</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>601</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>602</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>603</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>604</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>605</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>606</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>607</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>608</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>609</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>610</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>611</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>598</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>612</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>598</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>613</v>
+      </c>
+      <c r="B13" s="13">
+        <v>1500</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>614</v>
+      </c>
+      <c r="B14" s="13">
+        <v>1500</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>615</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>616</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>617</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>618</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>619</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>620</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>621</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>620</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
+        <v>622</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>623</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>593</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E00C0EE-B5EA-4C5D-A3F6-0409760A68CF}">
   <dimension ref="A1:B29"/>
   <sheetViews>
@@ -5319,7 +5647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD85EB1-BDB8-4AEB-99D1-57DF875DFEB5}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -5571,7 +5899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE4F375-28FB-4634-A90F-E29F4CD5ADA1}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -5824,7 +6152,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EA6128-27F4-4911-A1F0-865B26420EEF}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -6077,7 +6405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680EF845-E97A-4774-A116-33BCEE8AAAAA}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -6191,7 +6519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2A9967-94EA-41CF-ACB5-C81483AD239D}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -6296,151 +6624,6 @@
         <v>271</v>
       </c>
       <c r="B12" t="s">
-        <v>234</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2758D6-F888-4498-88A0-7DFBF7091CA2}">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="53.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>434</v>
-      </c>
-      <c r="B2">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>436</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>437</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>438</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>439</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>440</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>441</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="B10" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="B11" s="6"/>
-    </row>
-    <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="B13" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="B14" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B16" t="s">
         <v>234</v>
       </c>
     </row>
@@ -6610,6 +6793,151 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2758D6-F888-4498-88A0-7DFBF7091CA2}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="53.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B10" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B16" t="s">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ED34DA-E2CB-4859-9A96-48DF7AE0B7A7}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -6711,12 +7039,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F6BE80-AC56-42ED-87D6-9266FD24F810}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6848,7 +7176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA74624B-4AE3-43E9-9C9C-696C43DB0CE5}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -6963,12 +7291,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A321CDB-4432-42F8-8542-C3389F944EAE}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
use real question to construct output
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDSQuestionAnswer_2020_2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\irpa_db\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCDD8596-9AC9-4A8C-8367-519053A49505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B093560-F048-44D0-B284-D417613190DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="22" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -1471,15 +1471,6 @@
     <t xml:space="preserve">(xor [academic_factor] [non_academic_factor]) is &lt;value&gt; in Rose-Hulman admission decisions </t>
   </si>
   <si>
-    <t xml:space="preserve">The percentage of freshman students with sat composite score (xor {[range] [number] and [number]} {[range] [number]}) is &lt;value&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The percentage of freshman students with sat (xor [test_component] [subject]) score (xor {[range] [number] and [number]} {[range] [number]}) is &lt;value&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The percentage of freshman students with act (xor [test_component] [subject]) score (xor {[range] [number] and [number]} {[range] [number]}) is &lt;value&gt; </t>
-  </si>
-  <si>
     <t>How many freshman student submitted ACT</t>
   </si>
   <si>
@@ -1492,9 +1483,6 @@
     <t>What is the percent of freshman students submitting ACT</t>
   </si>
   <si>
-    <t>What is the percentage of freshman students with gpa between 4.00?</t>
-  </si>
-  <si>
     <t>What is the percentage of freshman students with gpa between 3.75 and 3.99?</t>
   </si>
   <si>
@@ -1547,9 +1535,6 @@
   </si>
   <si>
     <t>The percentage of freshman students who submitted gpa is 94.9 % (504/531)</t>
-  </si>
-  <si>
-    <t>The percentage of freshman students in the [class_rank] of their high school graduating class is &lt;value?</t>
   </si>
   <si>
     <t>What is the average need-based loan for students who were awarded any need-based self-help aid?</t>
@@ -1827,27 +1812,15 @@
     <t>How many degree-seeking first-time first-year american indians are enrolled?</t>
   </si>
   <si>
-    <t xml:space="preserve">The percentage of freshman students with act composite score (xor {[range] [number] and [number]} {[range] [number]}) is &lt;value&gt; </t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>The (xor [aggregation] [percentile]) score [standarized_test] [subject] for freshmen is &lt;value&gt;</t>
-  </si>
-  <si>
     <t>296</t>
   </si>
   <si>
-    <t>The (xor number [*percentage]) of freshman students who submitted [standarized_test] score is &lt;value&gt;</t>
-  </si>
-  <si>
     <t>28</t>
   </si>
   <si>
-    <t>The percentage of freshman students with gpa (xor {[range] [number] and [number]} {[range] [number]}) is &lt;value&gt;</t>
-  </si>
-  <si>
     <t>What is the URL of your institution's Net price calculator?</t>
   </si>
   <si>
@@ -1945,6 +1918,33 @@
   </si>
   <si>
     <t>per-credit-hour charges $1,444</t>
+  </si>
+  <si>
+    <t>The (xor number [^*percentage]) of freshman students who submitted [standarized_test] score is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The percentage of freshman students with act (xor [test_component] [subject]) score (xor {between [^number] and [^number]} {[^range] [^number]}) is &lt;value&gt; </t>
+  </si>
+  <si>
+    <t>The (xor [^aggregation] [^percentile]) score [standarized_test] [subject] for freshmen is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>The percentage of freshman students with gpa (xor {[^range] [^number] and [^number]} {[^range] [^number]}) is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>The percentage of freshman students in the [class_rank] of their high school graduating class is &lt;value&gt;?</t>
+  </si>
+  <si>
+    <t>What is the percentage of freshman students with gpa within 4.00?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The percentage of freshman students with act composite score (xor {between [^number] and [^number]} {[^range] [^number]}) is &lt;value&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The percentage of freshman students with sat (xor [test_component] [subject]) score (xor {between [^number] and [^number]} {[^range] [^number]}) is &lt;value&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The percentage of freshman students with sat composite score (xor {between [^number] and [^number]} {[^range] [^number]}) is &lt;value&gt; </t>
   </si>
 </sst>
 </file>
@@ -2007,7 +2007,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -2037,9 +2037,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2544,8 +2541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF2A7F2-CEC5-4907-876C-DED9EAEEDD17}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2628,7 +2625,7 @@
         <v>266</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>466</v>
+        <v>623</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2672,8 +2669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C307D05E-B833-4D75-9855-8E27A1B5E2C9}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView zoomScale="84" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2805,7 +2802,7 @@
         <v>266</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>467</v>
+        <v>622</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -2854,7 +2851,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2937,7 +2934,7 @@
         <v>266</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>584</v>
+        <v>621</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2982,7 +2979,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3114,7 +3111,7 @@
         <v>266</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>468</v>
+        <v>616</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -3125,7 +3122,7 @@
         <v>196</v>
       </c>
       <c r="D17" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -3163,7 +3160,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3182,7 +3179,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>60</v>
@@ -3190,7 +3187,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>61</v>
@@ -3198,7 +3195,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B4" s="6">
         <v>350</v>
@@ -3206,10 +3203,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3230,7 +3227,7 @@
         <v>266</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>588</v>
+        <v>615</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -3275,14 +3272,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3892E9F-E7EA-42B9-AE4C-1275BBD6A387}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView zoomScale="105" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="81.21875" customWidth="1"/>
-    <col min="2" max="2" width="74.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="85.88671875" style="4" customWidth="1"/>
     <col min="3" max="3" width="19.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3435,7 +3432,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -3569,7 +3566,7 @@
         <v>266</v>
       </c>
       <c r="B36" t="s">
-        <v>586</v>
+        <v>617</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -3615,7 +3612,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3638,7 +3635,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>473</v>
+        <v>620</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>98</v>
@@ -3649,7 +3646,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>99</v>
@@ -3660,7 +3657,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>100</v>
@@ -3671,7 +3668,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>101</v>
@@ -3682,7 +3679,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>102</v>
@@ -3693,7 +3690,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>103</v>
@@ -3704,7 +3701,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>109</v>
@@ -3715,7 +3712,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>109</v>
@@ -3726,7 +3723,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>109</v>
@@ -3737,10 +3734,10 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C11" t="s">
         <v>196</v>
@@ -3748,10 +3745,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C12" t="s">
         <v>196</v>
@@ -3776,7 +3773,7 @@
         <v>266</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>590</v>
+        <v>618</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -3825,7 +3822,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3844,7 +3841,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>122</v>
@@ -3852,7 +3849,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>123</v>
@@ -3860,7 +3857,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>124</v>
@@ -3868,7 +3865,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>125</v>
@@ -3876,7 +3873,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>109</v>
@@ -3884,7 +3881,7 @@
     </row>
     <row r="7" spans="1:2" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>126</v>
@@ -3908,7 +3905,7 @@
         <v>266</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>492</v>
+        <v>619</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4081,7 +4078,7 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>159</v>
@@ -4092,7 +4089,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>318</v>
@@ -4643,7 +4640,7 @@
         <v>266</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -5195,201 +5192,201 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="5" t="s">
+        <v>582</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>585</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>587</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>591</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C5" s="5" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>592</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="B6" s="5" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="C6" s="5" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>594</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B7" s="5" t="s">
         <v>595</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="C7" s="5" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>596</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B8" s="5" t="s">
         <v>597</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C8" s="5" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="B9" s="5" t="s">
         <v>599</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="C9" s="5" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>600</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="B10" s="5" t="s">
         <v>601</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="C10" s="5" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>602</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="B11" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>603</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B12" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>604</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="B13" s="5">
+        <v>1500</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>605</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B14" s="5">
+        <v>1500</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="B15" s="5" t="s">
         <v>607</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="C15" s="5" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>608</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="B16" s="5" t="s">
         <v>609</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="C16" s="5" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>610</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+      <c r="B17" s="5" t="s">
         <v>611</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>598</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
+      <c r="C17" s="5" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>612</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>598</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="B18" s="5" t="s">
+        <v>611</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>613</v>
       </c>
-      <c r="B13" s="13">
-        <v>1500</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="B19" s="5" t="s">
         <v>614</v>
       </c>
-      <c r="B14" s="13">
-        <v>1500</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
-        <v>615</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>616</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
-        <v>617</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>618</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>619</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>620</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
-        <v>621</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>620</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
-        <v>622</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>623</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>593</v>
+      <c r="C19" s="5" t="s">
+        <v>584</v>
       </c>
     </row>
   </sheetData>
@@ -5493,7 +5490,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>387</v>
@@ -5501,7 +5498,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>388</v>
@@ -5509,7 +5506,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>389</v>
@@ -5517,7 +5514,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>381</v>
@@ -5525,7 +5522,7 @@
     </row>
     <row r="15" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>381</v>
@@ -5533,7 +5530,7 @@
     </row>
     <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>381</v>
@@ -5606,7 +5603,7 @@
         <v>266</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -6048,7 +6045,7 @@
     </row>
     <row r="13" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>410</v>
@@ -6156,7 +6153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EA6128-27F4-4911-A1F0-865B26420EEF}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -6429,7 +6426,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="B2">
         <v>33</v>
@@ -6437,7 +6434,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -6445,7 +6442,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -6453,7 +6450,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -6478,7 +6475,7 @@
         <v>266</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -6592,7 +6589,7 @@
         <v>266</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -6744,7 +6741,7 @@
         <v>266</v>
       </c>
       <c r="B13" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -6784,7 +6781,7 @@
         <v>314</v>
       </c>
       <c r="B18" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
     </row>
   </sheetData>
@@ -6897,7 +6894,7 @@
         <v>266</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -6965,10 +6962,10 @@
     </row>
     <row r="2" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="C2" t="s">
         <v>196</v>
@@ -6979,7 +6976,7 @@
         <v>442</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="C3" t="s">
         <v>196</v>
@@ -7063,15 +7060,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="B2" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="B3">
         <v>76</v>
@@ -7079,7 +7076,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="B4">
         <v>216</v>
@@ -7087,7 +7084,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="B5">
         <v>129</v>
@@ -7095,7 +7092,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -7103,7 +7100,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -7111,7 +7108,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -7119,7 +7116,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -7200,7 +7197,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -7208,7 +7205,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="B3">
         <v>33</v>
@@ -7216,7 +7213,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -7224,7 +7221,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -7232,7 +7229,7 @@
     </row>
     <row r="6" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -7240,7 +7237,7 @@
     </row>
     <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -7248,7 +7245,7 @@
     </row>
     <row r="8" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -7319,79 +7316,79 @@
     </row>
     <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
   </sheetData>
@@ -7424,7 +7421,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -7432,7 +7429,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -7440,7 +7437,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -7448,7 +7445,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="B5">
         <v>356</v>
@@ -7456,7 +7453,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -7464,7 +7461,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="B7">
         <v>36</v>
@@ -7472,7 +7469,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -7480,7 +7477,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="B9">
         <v>31</v>
@@ -7488,7 +7485,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -7512,7 +7509,7 @@
         <v>266</v>
       </c>
       <c r="B13" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -7747,7 +7744,7 @@
         <v>266</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -7816,7 +7813,7 @@
     </row>
     <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="B2" s="5">
         <v>4</v>
@@ -7827,7 +7824,7 @@
     </row>
     <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="B3" s="5">
         <v>4</v>
@@ -7838,7 +7835,7 @@
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
@@ -7849,7 +7846,7 @@
     </row>
     <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="B5" s="5">
         <v>3</v>
@@ -7860,7 +7857,7 @@
     </row>
     <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="B6" s="5">
         <v>0</v>
@@ -7871,7 +7868,7 @@
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -7882,7 +7879,7 @@
     </row>
     <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -7893,7 +7890,7 @@
     </row>
     <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -7904,7 +7901,7 @@
     </row>
     <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="B10" s="5">
         <v>0</v>
@@ -7915,7 +7912,7 @@
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="B11" s="5">
         <v>0</v>
@@ -7926,7 +7923,7 @@
     </row>
     <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="B12" s="5">
         <v>0</v>
@@ -7937,10 +7934,10 @@
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="C13" t="s">
         <v>196</v>
@@ -7964,7 +7961,7 @@
         <v>266</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -8029,7 +8026,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -8037,7 +8034,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -8045,7 +8042,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -8053,7 +8050,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -8061,7 +8058,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -8069,7 +8066,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -8077,7 +8074,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -8085,7 +8082,7 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -8093,7 +8090,7 @@
     </row>
     <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -8101,7 +8098,7 @@
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -8109,7 +8106,7 @@
     </row>
     <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -8134,7 +8131,7 @@
         <v>266</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>